<commit_message>
Update E2E test files and workflow configuration
</commit_message>
<xml_diff>
--- a/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
+++ b/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3248B5C6-E586-48B2-8CB2-E5F28E754517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Results Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Automation Execution History" sheetId="2" r:id="rId2"/>
-    <sheet name="Automation QA Dashboard" sheetId="3" r:id="rId3"/>
-    <sheet name="Cross-Browser QA Dashboard" sheetId="4" r:id="rId4"/>
+    <sheet name="Test Results Summary" r:id="rId8" sheetId="5"/>
+    <sheet name="Automation QA Dashboard" r:id="rId9" sheetId="8"/>
+    <sheet name="Cross-Browser QA Dashboard" r:id="rId10" sheetId="9"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:C22"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="174">
   <si>
     <t>Test Results Summary - 2025-11-21 18:35:50</t>
   </si>
@@ -424,13 +424,144 @@
   </si>
   <si>
     <t>Cross-Browser Enhanced</t>
+  </si>
+  <si>
+    <t>Test Results Summary - 2025-11-22 22:31:50</t>
+  </si>
+  <si>
+    <t>Daily Status [2025-11-22]: FAILED (1 run)</t>
+  </si>
+  <si>
+    <t>Total: 2</t>
+  </si>
+  <si>
+    <t>Passed: 1</t>
+  </si>
+  <si>
+    <t>Failed: 1</t>
+  </si>
+  <si>
+    <t>Duration: 1m 2s</t>
+  </si>
+  <si>
+    <t>01KFoneLogin.feature</t>
+  </si>
+  <si>
+    <t>Login to KFONE Application and Find client with access to Profile Manager Application</t>
+  </si>
+  <si>
+    <t>User logs in to KFOne with standard credentials</t>
+  </si>
+  <si>
+    <t>Time: 22:31:50 | Total: 2 | Pass: 1 | Fail: 1</t>
+  </si>
+  <si>
+    <t>Exception: TimeoutException
+Message: no such element: Unable to locate element: {"method":"xpath","selector":"//div[contains(@class,'kfone-header')]"}
+  (Session info: chrome=133.0.6943.127)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Build info: version: '4.25.0', revision: '8a8aea2337'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.16'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [8d564e67fcda4540771e0fd7ff4b5939, findElement {value=//div[contains(@class,'kfone-header')], using=xpath}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 133.0.6943.127, chrome: {chromedriverVersion: 133.0.6943.141 (2a5d6da0d61..., userDataDir: C:\Job Mapping\e2e-automati...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50282}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50282/devtoo..., se:cdpVersion: 133.0.6943.127, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 8d564e67fcda4540771e0fd7ff4b5939
+Key Stack Trace:
+  at org.openqa.selenium.support.ui.WebDriverWait.timeoutException(WebDriverWait.java:84)
+  at org.openqa.selenium.support.ui.FluentWait.until(FluentWait.java:228)
+  at com.kfonetalentsuite.pageobjects.JobMapping.PO01_KFoneLogin.provide_non_sso_login_password_and_click_sign_in_button_in_kfone_login_page(PO01_KFoneLogin.java:297)</t>
+  </si>
+  <si>
+    <t>clm.user.one@testkfy.com</t>
+  </si>
+  <si>
+    <t>CLM Test Company 1</t>
+  </si>
+  <si>
+    <t>2025-11-22</t>
+  </si>
+  <si>
+    <t>22:31:50</t>
+  </si>
+  <si>
+    <t>Runner01_KFoneLogin</t>
+  </si>
+  <si>
+    <t>50.0%</t>
+  </si>
+  <si>
+    <t>1m 2s</t>
+  </si>
+  <si>
+    <t>Generated: 2025-11-22 22:31:50 | Environment: QA | Focus: Normal Single-Browser Execution</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>31.0s</t>
+  </si>
+  <si>
+    <t>2 of 332 (0.6%)</t>
+  </si>
+  <si>
+    <t>0.6%</t>
+  </si>
+  <si>
+    <t>2 scenarios</t>
+  </si>
+  <si>
+    <t>1 Passed</t>
+  </si>
+  <si>
+    <t>1 Failed</t>
+  </si>
+  <si>
+    <t>Generated: 2025-11-22 22:31:50 | Environment: QA | Focus: Cross-Browser Multi-Platform Execution</t>
+  </si>
+  <si>
+    <t>Test Results Summary - Last Updated: 2025-11-22 22:37:17</t>
+  </si>
+  <si>
+    <t>Daily Status [2025-11-22]: FAILED (2 runs)</t>
+  </si>
+  <si>
+    <t>Total: 4</t>
+  </si>
+  <si>
+    <t>Passed: 3</t>
+  </si>
+  <si>
+    <t>Duration: 1m 39s</t>
+  </si>
+  <si>
+    <t>Time: 22:37:17 | Total: 2 | Pass: 2 | Fail: 0</t>
+  </si>
+  <si>
+    <t>22:37:17</t>
+  </si>
+  <si>
+    <t>37s</t>
+  </si>
+  <si>
+    <t>Generated: 2025-11-22 22:37:17 | Environment: QA | Focus: Normal Single-Browser Execution</t>
+  </si>
+  <si>
+    <t>18.5s</t>
+  </si>
+  <si>
+    <t>2 Passed</t>
+  </si>
+  <si>
+    <t>Generated: 2025-11-22 22:37:17 | Environment: QA | Focus: Cross-Browser Multi-Platform Execution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="58" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="123" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -713,8 +844,346 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,8 +1235,63 @@
         <fgColor indexed="44"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="18"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="30"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="44"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -805,11 +1329,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -987,6 +1555,225 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="2" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="13" borderId="6" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="13" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="13" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="13" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="3" borderId="6" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="13" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="13" borderId="6" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="2" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="5" borderId="12" xfId="0" applyFont="true" applyFill="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="7" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="3" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="8" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="9" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="4" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="10" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="2" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="5" borderId="12" xfId="0" applyFont="true" applyFill="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="7" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="3" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="8" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="9" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="4" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="10" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="3" borderId="6" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="3" borderId="6" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="3" borderId="6" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="3" borderId="6" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="5" borderId="12" xfId="0" applyFont="true" applyFill="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="7" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="3" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="8" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="9" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="4" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="10" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="114" fillId="2" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="5" borderId="12" xfId="0" applyFont="true" applyFill="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="7" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="3" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="8" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="9" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="4" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="10" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1301,272 +2088,29 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="B6:B11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.3125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.4375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0078125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.24609375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.99609375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.4375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="37.40234375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.91015625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.96484375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="15.08984375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.5625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
@@ -1663,570 +2207,762 @@
         <v>18</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="78">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s" s="78">
+        <v>147</v>
+      </c>
+      <c r="C3" t="s" s="78">
+        <v>148</v>
+      </c>
+      <c r="D3" t="s" s="78">
+        <v>149</v>
+      </c>
+      <c r="E3" t="s" s="78">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s" s="78">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s" s="78">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s" s="78">
+        <v>150</v>
+      </c>
+      <c r="I3" t="n" s="78">
+        <v>2.0</v>
+      </c>
+      <c r="J3" t="n" s="78">
+        <v>1.0</v>
+      </c>
+      <c r="K3" t="n" s="78">
+        <v>1.0</v>
+      </c>
+      <c r="L3" t="n" s="78">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="s" s="78">
+        <v>151</v>
+      </c>
+      <c r="N3" t="s" s="78">
+        <v>152</v>
+      </c>
+      <c r="O3" t="s" s="79">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="114">
+        <v>146</v>
+      </c>
+      <c r="B4" t="s" s="114">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s" s="114">
+        <v>148</v>
+      </c>
+      <c r="D4" t="s" s="114">
+        <v>168</v>
+      </c>
+      <c r="E4" t="s" s="114">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s" s="114">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s" s="114">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s" s="114">
+        <v>150</v>
+      </c>
+      <c r="I4" t="n" s="114">
+        <v>2.0</v>
+      </c>
+      <c r="J4" t="n" s="114">
+        <v>2.0</v>
+      </c>
+      <c r="K4" t="n" s="114">
+        <v>0.0</v>
+      </c>
+      <c r="L4" t="n" s="114">
+        <v>0.0</v>
+      </c>
+      <c r="M4" t="s" s="114">
+        <v>50</v>
+      </c>
+      <c r="N4" t="s" s="114">
+        <v>169</v>
+      </c>
+      <c r="O4" t="s" s="115">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.328125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="69.60546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="43.28125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.7578125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.25390625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.7734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="34.109375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="255.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="61">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="61">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s" s="61">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="61">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s" s="61">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s" s="61">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s" s="61">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s" s="61">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s" s="61">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="111">
+        <v>141</v>
+      </c>
+      <c r="B6" t="s" s="113">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s" s="65">
+        <v>143</v>
+      </c>
+      <c r="D6" t="s" s="62">
+        <v>113</v>
+      </c>
+      <c r="E6" t="s" s="63">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s" s="64">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s" s="66">
+        <v>144</v>
+      </c>
+      <c r="H6" t="s" s="67">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="111">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s" s="113">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s" s="71">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s" s="68">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s" s="69">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s" s="70">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s" s="72">
+        <v>144</v>
+      </c>
+      <c r="H7" t="s" s="73">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="111">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s" s="113">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s" s="101">
+        <v>143</v>
+      </c>
+      <c r="D8" t="s" s="98">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s" s="99">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s" s="100">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s" s="102">
+        <v>167</v>
+      </c>
+      <c r="H8" t="s" s="103">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="111">
+        <v>141</v>
+      </c>
+      <c r="B9" t="s" s="113">
+        <v>142</v>
+      </c>
+      <c r="C9" t="s" s="107">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s" s="104">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s" s="105">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s" s="106">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s" s="108">
+        <v>167</v>
+      </c>
+      <c r="H9" t="s" s="109">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.46875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.84375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="22.19140625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.84375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.671875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="17.546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.84375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.671875" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+    <row r="1" ht="18.0" customHeight="true">
+      <c r="A1" t="s" s="117">
         <v>52</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-    </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-    </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57" t="s">
+    </row>
+    <row r="2" ht="18.0" customHeight="true">
+      <c r="A2" t="s" s="118">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" ht="18.0" customHeight="true">
+      <c r="A4" t="s" s="116">
         <v>54</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+    </row>
+    <row r="5" ht="18.0" customHeight="true">
+      <c r="A5" t="s" s="124">
         <v>55</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" t="s" s="119">
         <v>56</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" t="s" s="124">
         <v>57</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" t="s" s="119">
         <v>58</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" t="s" s="124">
         <v>59</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" t="s" s="119">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+    <row r="6" ht="18.0" customHeight="true">
+      <c r="A6" t="s" s="124">
         <v>61</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" t="s" s="119">
         <v>50</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" t="s" s="124">
         <v>62</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" t="s" s="119">
         <v>18</v>
       </c>
-      <c r="G6" s="46" t="s">
+      <c r="G6" t="s" s="124">
         <v>63</v>
       </c>
-      <c r="H6" s="45" t="s">
+      <c r="H6" t="s" s="123">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+    <row r="8" ht="18.0" customHeight="true">
+      <c r="A8" t="s" s="116">
         <v>65</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-    </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
+    </row>
+    <row r="9" ht="18.0" customHeight="true">
+      <c r="A9" t="s" s="124">
         <v>66</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" t="s" s="123">
         <v>67</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" t="s" s="124">
         <v>68</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" t="s" s="123">
         <v>69</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" t="s" s="124">
         <v>70</v>
       </c>
-      <c r="H9" s="44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46" t="s">
+      <c r="H9" t="s" s="122">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" ht="18.0" customHeight="true">
+      <c r="A10" t="s" s="124">
         <v>72</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" t="s" s="122">
         <v>73</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" t="s" s="124">
         <v>74</v>
       </c>
-      <c r="E10" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="46" t="s">
+      <c r="E10" t="s" s="122">
+        <v>156</v>
+      </c>
+      <c r="G10" t="s" s="124">
         <v>76</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="H10" t="s" s="123">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="46" t="s">
+    <row r="11" ht="18.0" customHeight="true">
+      <c r="A11" t="s" s="124">
         <v>78</v>
       </c>
-      <c r="B11" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="46" t="s">
+      <c r="B11" t="s" s="123">
+        <v>169</v>
+      </c>
+      <c r="D11" t="s" s="124">
         <v>79</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E11" t="s" s="122">
+        <v>157</v>
+      </c>
+      <c r="G11" t="s" s="124">
+        <v>81</v>
+      </c>
+      <c r="H11" t="s" s="122">
         <v>80</v>
       </c>
-      <c r="G11" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57" t="s">
+    </row>
+    <row r="13" ht="18.0" customHeight="true">
+      <c r="A13" t="s" s="116">
         <v>82</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-    </row>
-    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
+    </row>
+    <row r="14" ht="18.0" customHeight="true">
+      <c r="A14" t="s" s="124">
         <v>83</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" t="s" s="119">
+        <v>158</v>
+      </c>
+      <c r="D14" t="s" s="124">
+        <v>85</v>
+      </c>
+      <c r="E14" t="s" s="122">
         <v>84</v>
       </c>
-      <c r="D14" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
+    </row>
+    <row r="15" ht="18.0" customHeight="true">
+      <c r="A15" t="s" s="124">
         <v>87</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" t="s" s="122">
         <v>84</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" t="s" s="124">
         <v>88</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" t="s" s="121">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46" t="s">
+    <row r="16" ht="18.0" customHeight="true">
+      <c r="A16" t="s" s="124">
         <v>89</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="41" t="s">
+      <c r="B16" t="s" s="119">
+        <v>172</v>
+      </c>
+      <c r="D16" t="s" s="119">
         <v>91</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" t="s" s="119">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="57" t="s">
+    <row r="18" ht="18.0" customHeight="true">
+      <c r="A18" t="s" s="116">
         <v>93</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-    </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46" t="s">
+    </row>
+    <row r="19" ht="18.0" customHeight="true">
+      <c r="A19" t="s" s="124">
         <v>94</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" t="s" s="123">
         <v>95</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" t="s" s="124">
         <v>96</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E19" t="s" s="119">
         <v>97</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" t="s" s="124">
         <v>98</v>
       </c>
-      <c r="H19" s="41" t="s">
+      <c r="H19" t="s" s="119">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46" t="s">
+    <row r="20" ht="18.0" customHeight="true">
+      <c r="A20" t="s" s="124">
         <v>100</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" t="s" s="119">
         <v>101</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" t="s" s="124">
         <v>102</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" t="s" s="119">
         <v>103</v>
       </c>
-      <c r="G20" s="46" t="s">
+      <c r="G20" t="s" s="124">
         <v>104</v>
       </c>
-      <c r="H20" s="42" t="s">
+      <c r="H20" t="s" s="120">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A18:H18"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A18:H18"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.53125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.71875" customWidth="true"/>
+    <col min="4" max="4" width="19.53125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="17.578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.71875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="17.578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="17.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="126">
         <v>106</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-    </row>
-    <row r="4" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="60" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="127">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="125">
         <v>54</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="133">
         <v>108</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" t="s" s="131">
         <v>109</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" t="s" s="133">
         <v>110</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" t="s" s="131">
         <v>109</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" t="s" s="133">
         <v>59</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" t="s" s="131">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
+    <row r="6">
+      <c r="A6" t="s" s="133">
         <v>57</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" t="s" s="131">
         <v>112</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" t="s" s="133">
         <v>62</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" t="s" s="131">
         <v>113</v>
       </c>
-      <c r="G6" s="51" t="s">
+      <c r="G6" t="s" s="133">
         <v>63</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" t="s" s="128">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="60" t="s">
+    <row r="8">
+      <c r="A8" t="s" s="125">
         <v>65</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="51" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="133">
         <v>66</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" t="s" s="132">
         <v>67</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" t="s" s="133">
         <v>68</v>
       </c>
-      <c r="E9" s="50" t="s">
+      <c r="E9" t="s" s="132">
         <v>69</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G9" t="s" s="133">
         <v>115</v>
       </c>
-      <c r="H9" s="50" t="s">
+      <c r="H9" t="s" s="132">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="51" t="s">
+    <row r="10">
+      <c r="A10" t="s" s="133">
         <v>72</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" t="s" s="131">
         <v>117</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" t="s" s="133">
         <v>118</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" t="s" s="129">
         <v>119</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" t="s" s="133">
         <v>76</v>
       </c>
-      <c r="H10" s="50" t="s">
+      <c r="H10" t="s" s="132">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="s">
+    <row r="11">
+      <c r="A11" t="s" s="133">
         <v>78</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" t="s" s="132">
         <v>116</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" t="s" s="133">
         <v>120</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" t="s" s="128">
         <v>121</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G11" t="s" s="133">
         <v>122</v>
       </c>
-      <c r="H11" s="49" t="s">
+      <c r="H11" t="s" s="131">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A13" s="60" t="s">
+    <row r="13">
+      <c r="A13" t="s" s="125">
         <v>123</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="51" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="133">
         <v>124</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" t="s" s="132">
         <v>125</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" t="s" s="133">
         <v>126</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" t="s" s="132">
         <v>125</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" t="s" s="133">
         <v>127</v>
       </c>
-      <c r="H14" s="50" t="s">
+      <c r="H14" t="s" s="132">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="51" t="s">
+    <row r="15">
+      <c r="A15" t="s" s="133">
         <v>89</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" t="s" s="128">
         <v>128</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" t="s" s="128">
         <v>91</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" t="s" s="128">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="60" t="s">
+    <row r="17">
+      <c r="A17" t="s" s="125">
         <v>129</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="133">
         <v>130</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" t="s" s="128">
         <v>131</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" t="s" s="133">
         <v>96</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" t="s" s="128">
         <v>101</v>
       </c>
-      <c r="G18" s="51" t="s">
+      <c r="G18" t="s" s="133">
         <v>98</v>
       </c>
-      <c r="H18" s="48" t="s">
+      <c r="H18" t="s" s="129">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="51" t="s">
+    <row r="19">
+      <c r="A19" t="s" s="133">
         <v>132</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" t="s" s="128">
         <v>10</v>
       </c>
-      <c r="D19" s="51" t="s">
+      <c r="D19" t="s" s="133">
         <v>102</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" t="s" s="129">
         <v>133</v>
       </c>
-      <c r="G19" s="51" t="s">
+      <c r="G19" t="s" s="133">
         <v>104</v>
       </c>
-      <c r="H19" s="48" t="s">
+      <c r="H19" t="s" s="129">
         <v>134</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A17:H17"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A17:H17"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update test results and test suite configuration
</commit_message>
<xml_diff>
--- a/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
+++ b/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
@@ -8,34 +8,34 @@
   <sheets>
     <sheet name="Test Results Summary" r:id="rId3" sheetId="1"/>
     <sheet name="Automation Execution History" r:id="rId4" sheetId="2"/>
-    <sheet name="Automation QA Dashboard" r:id="rId5" sheetId="3"/>
-    <sheet name="Cross-Browser QA Dashboard" r:id="rId6" sheetId="4"/>
+    <sheet name="Automation QA Dashboard" r:id="rId7" sheetId="5"/>
+    <sheet name="Cross-Browser QA Dashboard" r:id="rId8" sheetId="6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="201">
-  <si>
-    <t>Test Results Summary - 2025-12-08 10:58:45</t>
-  </si>
-  <si>
-    <t>Daily Status [2025-12-08]: FAILED (1 run)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="218">
+  <si>
+    <t>Test Results Summary - 2025-12-08 12:05:36</t>
+  </si>
+  <si>
+    <t>Daily Status [2025-12-08]: PASSED (1 run)</t>
   </si>
   <si>
     <t>Total: 69</t>
   </si>
   <si>
-    <t>Passed: 68</t>
-  </si>
-  <si>
-    <t>Failed: 1</t>
+    <t>Passed: 69</t>
+  </si>
+  <si>
+    <t>Failed: 0</t>
   </si>
   <si>
     <t>Skipped: 0</t>
   </si>
   <si>
-    <t>Duration: 10m 32s</t>
+    <t>Duration: 12m 0s</t>
   </si>
   <si>
     <t>Feature File</t>
@@ -77,7 +77,7 @@
     <t/>
   </si>
   <si>
-    <t>Time: 10:58:45 | Total: 2 | Pass: 2 | Fail: 0</t>
+    <t>Time: 12:05:36 | Total: 2 | Pass: 2 | Fail: 0</t>
   </si>
   <si>
     <t>Test executed successfully</t>
@@ -92,7 +92,7 @@
     <t>Verify Components in Job Mapping Page</t>
   </si>
   <si>
-    <t>Time: 10:58:45 | Total: 16 | Pass: 16 | Fail: 0</t>
+    <t>Time: 12:05:36 | Total: 16 | Pass: 16 | Fail: 0</t>
   </si>
   <si>
     <t>Navigate to Job Mapping page</t>
@@ -143,7 +143,7 @@
     <t>Publishing job profiles from Job profile details popup</t>
   </si>
   <si>
-    <t>Time: 10:58:45 | Total: 7 | Pass: 7 | Fail: 0</t>
+    <t>Time: 12:05:36 | Total: 7 | Pass: 7 | Fail: 0</t>
   </si>
   <si>
     <t>User publishes job profile from the profile details popup</t>
@@ -182,7 +182,7 @@
     <t>Verify Info Message for Multiple Profiles with Missing Data</t>
   </si>
   <si>
-    <t>Time: 10:58:45 | Total: 9 | Pass: 9 | Fail: 0</t>
+    <t>Time: 12:05:36 | Total: 9 | Pass: 9 | Fail: 0</t>
   </si>
   <si>
     <t>Verify Info Message displays on first profile with missing data</t>
@@ -209,7 +209,7 @@
     <t>Validate Add More Jobs functionality in AI Auto Job Mapping Page</t>
   </si>
   <si>
-    <t>Time: 10:58:45 | Total: 6 | Pass: 6 | Fail: 0</t>
+    <t>Time: 12:05:36 | Total: 6 | Pass: 6 | Fail: 0</t>
   </si>
   <si>
     <t>User accesses job upload functionality through Add More Jobs button</t>
@@ -251,7 +251,7 @@
     <t>Validate HCM Sync Profiles screen functionality in PM</t>
   </si>
   <si>
-    <t>Time: 10:58:45 | Total: 13 | Pass: 12 | Fail: 1</t>
+    <t>Time: 12:05:36 | Total: 13 | Pass: 13 | Fail: 0</t>
   </si>
   <si>
     <t>Verify Title and Description of HCM Sync Profiles</t>
@@ -284,280 +284,273 @@
     <t>Verify Sync with HCM button is Enabled and Disabled based on profile selection and deselection respectively in HCM Sync Profiles screen</t>
   </si>
   <si>
+    <t>Verify Sync with HCM button functionality and Verify PopUp</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Client Name</t>
+  </si>
+  <si>
+    <t>Testing Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Execution Type</t>
+  </si>
+  <si>
+    <t>Browser Results</t>
+  </si>
+  <si>
+    <t>Runner / Suite File</t>
+  </si>
+  <si>
+    <t>Functions Tested</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Issues Found</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t>Success Rate</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Quality Status</t>
+  </si>
+  <si>
+    <t>AIAuto.user.one@kfdbhdevoutlook.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>AI AutoMap test Client</t>
+  </si>
+  <si>
+    <t>2025-12-08</t>
+  </si>
+  <si>
+    <t>12:05:36</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
+  <si>
+    <t>Job Mapping - Sanity Test Suite</t>
+  </si>
+  <si>
+    <t>100.0%</t>
+  </si>
+  <si>
+    <t>12m 0s</t>
+  </si>
+  <si>
+    <t>Job Mapping - NORMAL EXECUTION QA DASHBOARD</t>
+  </si>
+  <si>
+    <t>Generated: 2025-12-08 12:05:36 | Environment: QA | Focus: Normal Single-Browser Execution</t>
+  </si>
+  <si>
+    <t>EXECUTIVE SCORECARD</t>
+  </si>
+  <si>
+    <t>Health Score:</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>Risk Level:</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>Business Impact:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MINIMAL</t>
+  </si>
+  <si>
+    <t>Success Rate:</t>
+  </si>
+  <si>
+    <t>Critical Path:</t>
+  </si>
+  <si>
+    <t>Execution Mode:</t>
+  </si>
+  <si>
+    <t>Headless</t>
+  </si>
+  <si>
+    <t>PROJECT OVERVIEW</t>
+  </si>
+  <si>
+    <t>Total Features in Project:</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>Total Scenarios in Project:</t>
+  </si>
+  <si>
+    <t>346</t>
+  </si>
+  <si>
+    <t>Avg Execution Time:</t>
+  </si>
+  <si>
+    <t>10.4s</t>
+  </si>
+  <si>
+    <t>Features Executed:</t>
+  </si>
+  <si>
+    <t>1 of 57 (1.8%)</t>
+  </si>
+  <si>
+    <t>Scenarios Executed:</t>
+  </si>
+  <si>
+    <t>69 of 346 (19.9%)</t>
+  </si>
+  <si>
+    <t>Environment:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> QA</t>
+  </si>
+  <si>
+    <t>Total Duration:</t>
+  </si>
+  <si>
+    <t>Project Coverage:</t>
+  </si>
+  <si>
+    <t>19.9%</t>
+  </si>
+  <si>
+    <t>Feature Coverage:</t>
+  </si>
+  <si>
+    <t>1.8%</t>
+  </si>
+  <si>
+    <t>TEST COVERAGE ANALYTICS</t>
+  </si>
+  <si>
+    <t>Authentication:</t>
+  </si>
+  <si>
+    <t>0 scenarios</t>
+  </si>
+  <si>
+    <t>AI AutoMapping:</t>
+  </si>
+  <si>
+    <t>69 scenarios</t>
+  </si>
+  <si>
+    <t>Profile Management:</t>
+  </si>
+  <si>
+    <t>AutoAI Manual Mapping:</t>
+  </si>
+  <si>
+    <t>Results Breakdown:</t>
+  </si>
+  <si>
+    <t>69 Passed</t>
+  </si>
+  <si>
+    <t>0 Failed</t>
+  </si>
+  <si>
+    <t>0 Skipped</t>
+  </si>
+  <si>
+    <t>PERFORMANCE &amp; CONFIGURATION</t>
+  </si>
+  <si>
+    <t>Browser:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CHROME</t>
+  </si>
+  <si>
+    <t>Excel Reporting:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enabled</t>
+  </si>
+  <si>
+    <t>Framework Version:</t>
+  </si>
+  <si>
+    <t>v2.1.0</t>
+  </si>
+  <si>
+    <t>Screenshot Capture:</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Session Recovery:</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Page Objects:</t>
+  </si>
+  <si>
+    <t>24 Enhanced</t>
+  </si>
+  <si>
+    <t>Job Mapping - CROSS-BROWSER QA DASHBOARD</t>
+  </si>
+  <si>
+    <t>Generated: 2025-12-08 12:05:36 | Environment: QA | Focus: Cross-Browser Multi-Platform Execution</t>
+  </si>
+  <si>
+    <t>Compatibility Score:</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>Cross-Browser Success Rate:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HIGH</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
     <t>FAILED</t>
   </si>
   <si>
-    <t>Exception: AssertionError
-Message: Issue in verifying Sync with HCM button is disabled in HCM Sync Profiles screen in PM...Please Investigate!!!
-Key Stack Trace:
-  at org.testng.Assert.fail(Assert.java:111)
-  at com.kfonetalentsuite.pageobjects.JobMapping.PO22_ValidateHCMSyncProfilesScreen_PM.user_should_verify_sync_with_hcm_button_is_disabled_in_hcm_sync_profiles_tab(PO22_ValidateHCMSyncProfilesScreen_PM.java:1932)</t>
-  </si>
-  <si>
-    <t>Verify Sync with HCM button functionality and Verify PopUp</t>
-  </si>
-  <si>
-    <t>User Name</t>
-  </si>
-  <si>
-    <t>Client Name</t>
-  </si>
-  <si>
-    <t>Testing Date</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>Execution Type</t>
-  </si>
-  <si>
-    <t>Browser Results</t>
-  </si>
-  <si>
-    <t>Runner / Suite File</t>
-  </si>
-  <si>
-    <t>Functions Tested</t>
-  </si>
-  <si>
-    <t>Working</t>
-  </si>
-  <si>
-    <t>Issues Found</t>
-  </si>
-  <si>
-    <t>Skipped</t>
-  </si>
-  <si>
-    <t>Success Rate</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>Quality Status</t>
-  </si>
-  <si>
-    <t>AIAuto.user.one@kfdbhdevoutlook.onmicrosoft.com</t>
-  </si>
-  <si>
-    <t>AI AutoMap test Client</t>
-  </si>
-  <si>
-    <t>2025-12-08</t>
-  </si>
-  <si>
-    <t>10:58:45</t>
-  </si>
-  <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>CHROME</t>
-  </si>
-  <si>
-    <t>Job Mapping - Sanity Test Suite</t>
-  </si>
-  <si>
-    <t>99.0%</t>
-  </si>
-  <si>
-    <t>10m 32s</t>
-  </si>
-  <si>
-    <t>Job Mapping - NORMAL EXECUTION QA DASHBOARD</t>
-  </si>
-  <si>
-    <t>Generated: 2025-12-08 10:58:45 | Environment: QA | Focus: Normal Single-Browser Execution</t>
-  </si>
-  <si>
-    <t>EXECUTIVE SCORECARD</t>
-  </si>
-  <si>
-    <t>Health Score:</t>
-  </si>
-  <si>
-    <t>100%</t>
-  </si>
-  <si>
-    <t>Risk Level:</t>
-  </si>
-  <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>Business Impact:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MINIMAL</t>
-  </si>
-  <si>
-    <t>Success Rate:</t>
-  </si>
-  <si>
-    <t>Critical Path:</t>
-  </si>
-  <si>
-    <t>Execution Mode:</t>
-  </si>
-  <si>
-    <t>Headless</t>
-  </si>
-  <si>
-    <t>PROJECT OVERVIEW</t>
-  </si>
-  <si>
-    <t>Total Features in Project:</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>Total Scenarios in Project:</t>
-  </si>
-  <si>
-    <t>346</t>
-  </si>
-  <si>
-    <t>Avg Execution Time:</t>
-  </si>
-  <si>
-    <t>9.2s</t>
-  </si>
-  <si>
-    <t>Features Executed:</t>
-  </si>
-  <si>
-    <t>1 of 57 (1.8%)</t>
-  </si>
-  <si>
-    <t>Scenarios Executed:</t>
-  </si>
-  <si>
-    <t>69 of 346 (19.9%)</t>
-  </si>
-  <si>
-    <t>Environment:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> QA</t>
-  </si>
-  <si>
-    <t>Total Duration:</t>
-  </si>
-  <si>
-    <t>Project Coverage:</t>
-  </si>
-  <si>
-    <t>19.9%</t>
-  </si>
-  <si>
-    <t>Feature Coverage:</t>
-  </si>
-  <si>
-    <t>1.8%</t>
-  </si>
-  <si>
-    <t>TEST COVERAGE ANALYTICS</t>
-  </si>
-  <si>
-    <t>Authentication:</t>
-  </si>
-  <si>
-    <t>0 scenarios</t>
-  </si>
-  <si>
-    <t>AI AutoMapping:</t>
-  </si>
-  <si>
-    <t>69 scenarios</t>
-  </si>
-  <si>
-    <t>Profile Management:</t>
-  </si>
-  <si>
-    <t>AutoAI Manual Mapping:</t>
-  </si>
-  <si>
-    <t>Results Breakdown:</t>
-  </si>
-  <si>
-    <t>68 Passed</t>
-  </si>
-  <si>
-    <t>1 Failed</t>
-  </si>
-  <si>
-    <t>0 Skipped</t>
-  </si>
-  <si>
-    <t>PERFORMANCE &amp; CONFIGURATION</t>
-  </si>
-  <si>
-    <t>Browser:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CHROME</t>
-  </si>
-  <si>
-    <t>Excel Reporting:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enabled</t>
-  </si>
-  <si>
-    <t>Framework Version:</t>
-  </si>
-  <si>
-    <t>v2.1.0</t>
-  </si>
-  <si>
-    <t>Screenshot Capture:</t>
-  </si>
-  <si>
-    <t>Enabled</t>
-  </si>
-  <si>
-    <t>Session Recovery:</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Page Objects:</t>
-  </si>
-  <si>
-    <t>24 Enhanced</t>
-  </si>
-  <si>
-    <t>Job Mapping - CROSS-BROWSER QA DASHBOARD</t>
-  </si>
-  <si>
-    <t>Generated: 2025-12-08 10:58:45 | Environment: QA | Focus: Cross-Browser Multi-Platform Execution</t>
-  </si>
-  <si>
-    <t>Compatibility Score:</t>
-  </si>
-  <si>
-    <t>0.0%</t>
-  </si>
-  <si>
-    <t>Cross-Browser Success Rate:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> HIGH</t>
-  </si>
-  <si>
-    <t>HIGH</t>
-  </si>
-  <si>
     <t>Cross-Browser</t>
   </si>
   <si>
@@ -603,9 +596,6 @@
     <t>0 Passed</t>
   </si>
   <si>
-    <t>0 Failed</t>
-  </si>
-  <si>
     <t>CROSS-BROWSER PERFORMANCE &amp; CONFIGURATION</t>
   </si>
   <si>
@@ -622,6 +612,63 @@
   </si>
   <si>
     <t>Cross-Browser Enhanced</t>
+  </si>
+  <si>
+    <t>Test Results Summary - Last Updated: 2025-12-08 15:01:48</t>
+  </si>
+  <si>
+    <t>Daily Status [2025-12-08]: ALL_PASSED (2 runs)</t>
+  </si>
+  <si>
+    <t>Total: 76</t>
+  </si>
+  <si>
+    <t>Passed: 76</t>
+  </si>
+  <si>
+    <t>Duration: 15m 19s</t>
+  </si>
+  <si>
+    <t>Time: 15:01:48 | Total: 7 | Pass: 7 | Fail: 0</t>
+  </si>
+  <si>
+    <t>15:01:48</t>
+  </si>
+  <si>
+    <t>Runner11c_ValidateFunctionSubfunctionFilters</t>
+  </si>
+  <si>
+    <t>3m 19s</t>
+  </si>
+  <si>
+    <t>Generated: 2025-12-08 15:01:48 | Environment: QA | Focus: Normal Single-Browser Execution</t>
+  </si>
+  <si>
+    <t>12.1s</t>
+  </si>
+  <si>
+    <t>2 of 57 (3.5%)</t>
+  </si>
+  <si>
+    <t>76 of 346 (22.0%)</t>
+  </si>
+  <si>
+    <t>15m 19s</t>
+  </si>
+  <si>
+    <t>22.0%</t>
+  </si>
+  <si>
+    <t>3.5%</t>
+  </si>
+  <si>
+    <t>76 scenarios</t>
+  </si>
+  <si>
+    <t>76 Passed</t>
+  </si>
+  <si>
+    <t>Generated: 2025-12-08 15:01:48 | Environment: QA | Focus: Cross-Browser Multi-Platform Execution</t>
   </si>
 </sst>
 </file>
@@ -629,7 +676,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="437">
+  <fonts count="499">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -2389,7 +2436,7 @@
       <name val="Arial"/>
       <sz val="10.0"/>
       <b val="true"/>
-      <color indexed="16"/>
+      <color indexed="58"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -2450,7 +2497,303 @@
       <name val="Arial"/>
       <sz val="10.0"/>
       <b val="true"/>
-      <color indexed="16"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -2721,7 +3064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="441">
+  <cellXfs count="507">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
@@ -3932,7 +4275,7 @@
     <xf numFmtId="0" fontId="403" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="404" fillId="7" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="404" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="405" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
@@ -3941,13 +4284,13 @@
     <xf numFmtId="0" fontId="406" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="407" fillId="7" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="408" fillId="7" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="409" fillId="7" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+    <xf numFmtId="0" fontId="407" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="408" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="409" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="410" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
@@ -3983,10 +4326,10 @@
     <xf numFmtId="0" fontId="416" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="417" fillId="7" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="418" fillId="7" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="417" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="418" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="419" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
@@ -4041,6 +4384,204 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="436" fillId="21" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="437" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="438" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="439" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="440" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="441" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="442" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="443" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="444" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="445" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="446" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="447" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="448" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="449" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="450" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="451" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="452" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="453" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="454" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="455" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="456" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="457" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="458" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="459" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="460" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="461" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="462" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="463" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="464" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="465" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="466" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="467" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="468" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="469" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="470" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="471" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="472" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="473" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="474" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="475" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="476" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="477" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="478" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="479" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="480" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="481" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="482" fillId="11" borderId="10" xfId="0" applyFont="true" applyFill="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="483" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="484" fillId="15" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="485" fillId="5" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="486" fillId="17" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="487" fillId="19" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="488" fillId="9" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="489" fillId="21" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="490" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="491" fillId="11" borderId="10" xfId="0" applyFont="true" applyFill="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="492" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="493" fillId="15" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="494" fillId="5" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="495" fillId="17" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="496" fillId="19" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="497" fillId="9" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="498" fillId="21" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4049,36 +4590,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="46.08203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="69.60546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="110.77734375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="8.7578125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="9.25390625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="36.10546875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="188.25" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="59.13671875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="110.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.7578125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.25390625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.7734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="36.10546875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.34375"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>0</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>2</v>
+        <v>201</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>3</v>
+        <v>202</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>4</v>
@@ -4087,7 +4628,7 @@
         <v>5</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>6</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5">
@@ -4117,10 +4658,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="416">
+      <c r="A6" t="s" s="483">
         <v>15</v>
       </c>
-      <c r="B6" t="s" s="418">
+      <c r="B6" t="s" s="485">
         <v>16</v>
       </c>
       <c r="C6" t="s" s="5">
@@ -4143,10 +4684,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="416">
+      <c r="A7" t="s" s="483">
         <v>15</v>
       </c>
-      <c r="B7" t="s" s="418">
+      <c r="B7" t="s" s="485">
         <v>16</v>
       </c>
       <c r="C7" t="s" s="11">
@@ -4169,10 +4710,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="416">
+      <c r="A8" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B8" t="s" s="418">
+      <c r="B8" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C8" t="s" s="17">
@@ -4195,10 +4736,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="416">
+      <c r="A9" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B9" t="s" s="418">
+      <c r="B9" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C9" t="s" s="23">
@@ -4221,10 +4762,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="416">
+      <c r="A10" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B10" t="s" s="418">
+      <c r="B10" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C10" t="s" s="29">
@@ -4247,10 +4788,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="416">
+      <c r="A11" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B11" t="s" s="418">
+      <c r="B11" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C11" t="s" s="35">
@@ -4273,10 +4814,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s" s="416">
+      <c r="A12" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B12" t="s" s="418">
+      <c r="B12" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C12" t="s" s="41">
@@ -4299,10 +4840,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="416">
+      <c r="A13" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B13" t="s" s="418">
+      <c r="B13" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C13" t="s" s="47">
@@ -4325,10 +4866,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="416">
+      <c r="A14" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B14" t="s" s="418">
+      <c r="B14" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C14" t="s" s="53">
@@ -4351,10 +4892,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="416">
+      <c r="A15" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B15" t="s" s="418">
+      <c r="B15" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C15" t="s" s="59">
@@ -4377,10 +4918,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s" s="416">
+      <c r="A16" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B16" t="s" s="418">
+      <c r="B16" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C16" t="s" s="65">
@@ -4403,10 +4944,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="416">
+      <c r="A17" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B17" t="s" s="418">
+      <c r="B17" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C17" t="s" s="71">
@@ -4429,10 +4970,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s" s="416">
+      <c r="A18" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B18" t="s" s="418">
+      <c r="B18" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C18" t="s" s="77">
@@ -4455,10 +4996,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="416">
+      <c r="A19" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B19" t="s" s="418">
+      <c r="B19" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C19" t="s" s="83">
@@ -4481,10 +5022,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s" s="416">
+      <c r="A20" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B20" t="s" s="418">
+      <c r="B20" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C20" t="s" s="89">
@@ -4507,10 +5048,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s" s="416">
+      <c r="A21" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B21" t="s" s="418">
+      <c r="B21" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C21" t="s" s="95">
@@ -4533,10 +5074,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s" s="416">
+      <c r="A22" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B22" t="s" s="418">
+      <c r="B22" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C22" t="s" s="101">
@@ -4559,10 +5100,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s" s="416">
+      <c r="A23" t="s" s="483">
         <v>23</v>
       </c>
-      <c r="B23" t="s" s="418">
+      <c r="B23" t="s" s="485">
         <v>24</v>
       </c>
       <c r="C23" t="s" s="107">
@@ -4585,10 +5126,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s" s="416">
+      <c r="A24" t="s" s="483">
         <v>40</v>
       </c>
-      <c r="B24" t="s" s="418">
+      <c r="B24" t="s" s="485">
         <v>41</v>
       </c>
       <c r="C24" t="s" s="113">
@@ -4611,10 +5152,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="416">
+      <c r="A25" t="s" s="483">
         <v>40</v>
       </c>
-      <c r="B25" t="s" s="418">
+      <c r="B25" t="s" s="485">
         <v>41</v>
       </c>
       <c r="C25" t="s" s="119">
@@ -4637,10 +5178,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s" s="416">
+      <c r="A26" t="s" s="483">
         <v>40</v>
       </c>
-      <c r="B26" t="s" s="418">
+      <c r="B26" t="s" s="485">
         <v>41</v>
       </c>
       <c r="C26" t="s" s="125">
@@ -4663,10 +5204,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="416">
+      <c r="A27" t="s" s="483">
         <v>40</v>
       </c>
-      <c r="B27" t="s" s="418">
+      <c r="B27" t="s" s="485">
         <v>41</v>
       </c>
       <c r="C27" t="s" s="131">
@@ -4689,10 +5230,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s" s="416">
+      <c r="A28" t="s" s="483">
         <v>40</v>
       </c>
-      <c r="B28" t="s" s="418">
+      <c r="B28" t="s" s="485">
         <v>41</v>
       </c>
       <c r="C28" t="s" s="137">
@@ -4715,10 +5256,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s" s="416">
+      <c r="A29" t="s" s="483">
         <v>40</v>
       </c>
-      <c r="B29" t="s" s="418">
+      <c r="B29" t="s" s="485">
         <v>41</v>
       </c>
       <c r="C29" t="s" s="143">
@@ -4741,10 +5282,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s" s="416">
+      <c r="A30" t="s" s="483">
         <v>40</v>
       </c>
-      <c r="B30" t="s" s="418">
+      <c r="B30" t="s" s="485">
         <v>41</v>
       </c>
       <c r="C30" t="s" s="149">
@@ -4767,10 +5308,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s" s="416">
+      <c r="A31" t="s" s="483">
         <v>47</v>
       </c>
-      <c r="B31" t="s" s="418">
+      <c r="B31" t="s" s="485">
         <v>48</v>
       </c>
       <c r="C31" t="s" s="155">
@@ -4793,10 +5334,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s" s="416">
+      <c r="A32" t="s" s="483">
         <v>47</v>
       </c>
-      <c r="B32" t="s" s="418">
+      <c r="B32" t="s" s="485">
         <v>48</v>
       </c>
       <c r="C32" t="s" s="161">
@@ -4819,10 +5360,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s" s="416">
+      <c r="A33" t="s" s="483">
         <v>47</v>
       </c>
-      <c r="B33" t="s" s="418">
+      <c r="B33" t="s" s="485">
         <v>48</v>
       </c>
       <c r="C33" t="s" s="167">
@@ -4845,10 +5386,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s" s="416">
+      <c r="A34" t="s" s="483">
         <v>47</v>
       </c>
-      <c r="B34" t="s" s="418">
+      <c r="B34" t="s" s="485">
         <v>48</v>
       </c>
       <c r="C34" t="s" s="173">
@@ -4871,10 +5412,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s" s="416">
+      <c r="A35" t="s" s="483">
         <v>47</v>
       </c>
-      <c r="B35" t="s" s="418">
+      <c r="B35" t="s" s="485">
         <v>48</v>
       </c>
       <c r="C35" t="s" s="179">
@@ -4897,10 +5438,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s" s="416">
+      <c r="A36" t="s" s="483">
         <v>47</v>
       </c>
-      <c r="B36" t="s" s="418">
+      <c r="B36" t="s" s="485">
         <v>48</v>
       </c>
       <c r="C36" t="s" s="185">
@@ -4923,10 +5464,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s" s="416">
+      <c r="A37" t="s" s="483">
         <v>47</v>
       </c>
-      <c r="B37" t="s" s="418">
+      <c r="B37" t="s" s="485">
         <v>48</v>
       </c>
       <c r="C37" t="s" s="191">
@@ -4949,10 +5490,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s" s="416">
+      <c r="A38" t="s" s="483">
         <v>53</v>
       </c>
-      <c r="B38" t="s" s="418">
+      <c r="B38" t="s" s="485">
         <v>54</v>
       </c>
       <c r="C38" t="s" s="197">
@@ -4975,10 +5516,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s" s="416">
+      <c r="A39" t="s" s="483">
         <v>53</v>
       </c>
-      <c r="B39" t="s" s="418">
+      <c r="B39" t="s" s="485">
         <v>54</v>
       </c>
       <c r="C39" t="s" s="203">
@@ -5001,10 +5542,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s" s="416">
+      <c r="A40" t="s" s="483">
         <v>53</v>
       </c>
-      <c r="B40" t="s" s="418">
+      <c r="B40" t="s" s="485">
         <v>54</v>
       </c>
       <c r="C40" t="s" s="209">
@@ -5027,10 +5568,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s" s="416">
+      <c r="A41" t="s" s="483">
         <v>53</v>
       </c>
-      <c r="B41" t="s" s="418">
+      <c r="B41" t="s" s="485">
         <v>54</v>
       </c>
       <c r="C41" t="s" s="215">
@@ -5053,10 +5594,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s" s="416">
+      <c r="A42" t="s" s="483">
         <v>53</v>
       </c>
-      <c r="B42" t="s" s="418">
+      <c r="B42" t="s" s="485">
         <v>54</v>
       </c>
       <c r="C42" t="s" s="221">
@@ -5079,10 +5620,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s" s="416">
+      <c r="A43" t="s" s="483">
         <v>53</v>
       </c>
-      <c r="B43" t="s" s="418">
+      <c r="B43" t="s" s="485">
         <v>54</v>
       </c>
       <c r="C43" t="s" s="227">
@@ -5105,10 +5646,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s" s="416">
+      <c r="A44" t="s" s="483">
         <v>53</v>
       </c>
-      <c r="B44" t="s" s="418">
+      <c r="B44" t="s" s="485">
         <v>54</v>
       </c>
       <c r="C44" t="s" s="233">
@@ -5131,10 +5672,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s" s="416">
+      <c r="A45" t="s" s="483">
         <v>53</v>
       </c>
-      <c r="B45" t="s" s="418">
+      <c r="B45" t="s" s="485">
         <v>54</v>
       </c>
       <c r="C45" t="s" s="239">
@@ -5157,10 +5698,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s" s="416">
+      <c r="A46" t="s" s="483">
         <v>53</v>
       </c>
-      <c r="B46" t="s" s="418">
+      <c r="B46" t="s" s="485">
         <v>54</v>
       </c>
       <c r="C46" t="s" s="245">
@@ -5183,10 +5724,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s" s="416">
+      <c r="A47" t="s" s="483">
         <v>62</v>
       </c>
-      <c r="B47" t="s" s="418">
+      <c r="B47" t="s" s="485">
         <v>63</v>
       </c>
       <c r="C47" t="s" s="251">
@@ -5209,10 +5750,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s" s="416">
+      <c r="A48" t="s" s="483">
         <v>62</v>
       </c>
-      <c r="B48" t="s" s="418">
+      <c r="B48" t="s" s="485">
         <v>63</v>
       </c>
       <c r="C48" t="s" s="257">
@@ -5235,10 +5776,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s" s="416">
+      <c r="A49" t="s" s="483">
         <v>62</v>
       </c>
-      <c r="B49" t="s" s="418">
+      <c r="B49" t="s" s="485">
         <v>63</v>
       </c>
       <c r="C49" t="s" s="263">
@@ -5261,10 +5802,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s" s="416">
+      <c r="A50" t="s" s="483">
         <v>62</v>
       </c>
-      <c r="B50" t="s" s="418">
+      <c r="B50" t="s" s="485">
         <v>63</v>
       </c>
       <c r="C50" t="s" s="269">
@@ -5287,10 +5828,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s" s="416">
+      <c r="A51" t="s" s="483">
         <v>62</v>
       </c>
-      <c r="B51" t="s" s="418">
+      <c r="B51" t="s" s="485">
         <v>63</v>
       </c>
       <c r="C51" t="s" s="275">
@@ -5313,10 +5854,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s" s="416">
+      <c r="A52" t="s" s="483">
         <v>62</v>
       </c>
-      <c r="B52" t="s" s="418">
+      <c r="B52" t="s" s="485">
         <v>63</v>
       </c>
       <c r="C52" t="s" s="281">
@@ -5339,10 +5880,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="s" s="416">
+      <c r="A53" t="s" s="483">
         <v>68</v>
       </c>
-      <c r="B53" t="s" s="418">
+      <c r="B53" t="s" s="485">
         <v>69</v>
       </c>
       <c r="C53" t="s" s="287">
@@ -5365,10 +5906,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="s" s="416">
+      <c r="A54" t="s" s="483">
         <v>68</v>
       </c>
-      <c r="B54" t="s" s="418">
+      <c r="B54" t="s" s="485">
         <v>69</v>
       </c>
       <c r="C54" t="s" s="293">
@@ -5391,10 +5932,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="s" s="416">
+      <c r="A55" t="s" s="483">
         <v>68</v>
       </c>
-      <c r="B55" t="s" s="418">
+      <c r="B55" t="s" s="485">
         <v>69</v>
       </c>
       <c r="C55" t="s" s="299">
@@ -5417,10 +5958,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="s" s="416">
+      <c r="A56" t="s" s="483">
         <v>68</v>
       </c>
-      <c r="B56" t="s" s="418">
+      <c r="B56" t="s" s="485">
         <v>69</v>
       </c>
       <c r="C56" t="s" s="305">
@@ -5443,10 +5984,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="s" s="416">
+      <c r="A57" t="s" s="483">
         <v>68</v>
       </c>
-      <c r="B57" t="s" s="418">
+      <c r="B57" t="s" s="485">
         <v>69</v>
       </c>
       <c r="C57" t="s" s="311">
@@ -5469,10 +6010,10 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="s" s="416">
+      <c r="A58" t="s" s="483">
         <v>68</v>
       </c>
-      <c r="B58" t="s" s="418">
+      <c r="B58" t="s" s="485">
         <v>69</v>
       </c>
       <c r="C58" t="s" s="317">
@@ -5495,10 +6036,10 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s" s="416">
+      <c r="A59" t="s" s="483">
         <v>68</v>
       </c>
-      <c r="B59" t="s" s="418">
+      <c r="B59" t="s" s="485">
         <v>69</v>
       </c>
       <c r="C59" t="s" s="323">
@@ -5521,10 +6062,10 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s" s="416">
+      <c r="A60" t="s" s="483">
         <v>68</v>
       </c>
-      <c r="B60" t="s" s="418">
+      <c r="B60" t="s" s="485">
         <v>69</v>
       </c>
       <c r="C60" t="s" s="329">
@@ -5547,10 +6088,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="s" s="416">
+      <c r="A61" t="s" s="483">
         <v>68</v>
       </c>
-      <c r="B61" t="s" s="418">
+      <c r="B61" t="s" s="485">
         <v>69</v>
       </c>
       <c r="C61" t="s" s="335">
@@ -5573,10 +6114,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="s" s="417">
+      <c r="A62" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B62" t="s" s="419">
+      <c r="B62" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C62" t="s" s="341">
@@ -5599,10 +6140,10 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s" s="417">
+      <c r="A63" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B63" t="s" s="419">
+      <c r="B63" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C63" t="s" s="347">
@@ -5625,10 +6166,10 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="s" s="417">
+      <c r="A64" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B64" t="s" s="419">
+      <c r="B64" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C64" t="s" s="353">
@@ -5651,10 +6192,10 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s" s="417">
+      <c r="A65" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B65" t="s" s="419">
+      <c r="B65" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C65" t="s" s="359">
@@ -5677,10 +6218,10 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s" s="417">
+      <c r="A66" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B66" t="s" s="419">
+      <c r="B66" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C66" t="s" s="365">
@@ -5703,10 +6244,10 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s" s="417">
+      <c r="A67" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B67" t="s" s="419">
+      <c r="B67" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C67" t="s" s="371">
@@ -5729,10 +6270,10 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s" s="417">
+      <c r="A68" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B68" t="s" s="419">
+      <c r="B68" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C68" t="s" s="377">
@@ -5755,10 +6296,10 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="s" s="417">
+      <c r="A69" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B69" t="s" s="419">
+      <c r="B69" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C69" t="s" s="383">
@@ -5781,10 +6322,10 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="s" s="417">
+      <c r="A70" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B70" t="s" s="419">
+      <c r="B70" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C70" t="s" s="389">
@@ -5807,10 +6348,10 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="s" s="417">
+      <c r="A71" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B71" t="s" s="419">
+      <c r="B71" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C71" t="s" s="395">
@@ -5833,10 +6374,10 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="s" s="417">
+      <c r="A72" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B72" t="s" s="419">
+      <c r="B72" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C72" t="s" s="401">
@@ -5859,17 +6400,17 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="s" s="417">
+      <c r="A73" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B73" t="s" s="419">
+      <c r="B73" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C73" t="s" s="407">
         <v>88</v>
       </c>
       <c r="D73" t="s" s="404">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="E73" t="s" s="405">
         <v>19</v>
@@ -5881,18 +6422,18 @@
         <v>78</v>
       </c>
       <c r="H73" t="s" s="409">
-        <v>90</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="s" s="417">
+      <c r="A74" t="s" s="483">
         <v>76</v>
       </c>
-      <c r="B74" t="s" s="419">
+      <c r="B74" t="s" s="485">
         <v>77</v>
       </c>
       <c r="C74" t="s" s="413">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D74" t="s" s="410">
         <v>18</v>
@@ -5910,8 +6451,190 @@
         <v>21</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="s" s="483">
+        <v>47</v>
+      </c>
+      <c r="B75" t="s" s="485">
+        <v>48</v>
+      </c>
+      <c r="C75" t="s" s="444">
+        <v>17</v>
+      </c>
+      <c r="D75" t="s" s="441">
+        <v>18</v>
+      </c>
+      <c r="E75" t="s" s="442">
+        <v>19</v>
+      </c>
+      <c r="F75" t="s" s="443">
+        <v>19</v>
+      </c>
+      <c r="G75" t="s" s="445">
+        <v>204</v>
+      </c>
+      <c r="H75" t="s" s="446">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="483">
+        <v>47</v>
+      </c>
+      <c r="B76" t="s" s="485">
+        <v>48</v>
+      </c>
+      <c r="C76" t="s" s="450">
+        <v>22</v>
+      </c>
+      <c r="D76" t="s" s="447">
+        <v>18</v>
+      </c>
+      <c r="E76" t="s" s="448">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s" s="449">
+        <v>19</v>
+      </c>
+      <c r="G76" t="s" s="451">
+        <v>204</v>
+      </c>
+      <c r="H76" t="s" s="452">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="483">
+        <v>47</v>
+      </c>
+      <c r="B77" t="s" s="485">
+        <v>48</v>
+      </c>
+      <c r="C77" t="s" s="456">
+        <v>26</v>
+      </c>
+      <c r="D77" t="s" s="453">
+        <v>18</v>
+      </c>
+      <c r="E77" t="s" s="454">
+        <v>19</v>
+      </c>
+      <c r="F77" t="s" s="455">
+        <v>19</v>
+      </c>
+      <c r="G77" t="s" s="457">
+        <v>204</v>
+      </c>
+      <c r="H77" t="s" s="458">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="483">
+        <v>47</v>
+      </c>
+      <c r="B78" t="s" s="485">
+        <v>48</v>
+      </c>
+      <c r="C78" t="s" s="462">
+        <v>49</v>
+      </c>
+      <c r="D78" t="s" s="459">
+        <v>18</v>
+      </c>
+      <c r="E78" t="s" s="460">
+        <v>19</v>
+      </c>
+      <c r="F78" t="s" s="461">
+        <v>19</v>
+      </c>
+      <c r="G78" t="s" s="463">
+        <v>204</v>
+      </c>
+      <c r="H78" t="s" s="464">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="483">
+        <v>47</v>
+      </c>
+      <c r="B79" t="s" s="485">
+        <v>48</v>
+      </c>
+      <c r="C79" t="s" s="468">
+        <v>50</v>
+      </c>
+      <c r="D79" t="s" s="465">
+        <v>18</v>
+      </c>
+      <c r="E79" t="s" s="466">
+        <v>19</v>
+      </c>
+      <c r="F79" t="s" s="467">
+        <v>19</v>
+      </c>
+      <c r="G79" t="s" s="469">
+        <v>204</v>
+      </c>
+      <c r="H79" t="s" s="470">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="483">
+        <v>47</v>
+      </c>
+      <c r="B80" t="s" s="485">
+        <v>48</v>
+      </c>
+      <c r="C80" t="s" s="474">
+        <v>51</v>
+      </c>
+      <c r="D80" t="s" s="471">
+        <v>18</v>
+      </c>
+      <c r="E80" t="s" s="472">
+        <v>19</v>
+      </c>
+      <c r="F80" t="s" s="473">
+        <v>19</v>
+      </c>
+      <c r="G80" t="s" s="475">
+        <v>204</v>
+      </c>
+      <c r="H80" t="s" s="476">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="483">
+        <v>47</v>
+      </c>
+      <c r="B81" t="s" s="485">
+        <v>48</v>
+      </c>
+      <c r="C81" t="s" s="480">
+        <v>52</v>
+      </c>
+      <c r="D81" t="s" s="477">
+        <v>18</v>
+      </c>
+      <c r="E81" t="s" s="478">
+        <v>19</v>
+      </c>
+      <c r="F81" t="s" s="479">
+        <v>19</v>
+      </c>
+      <c r="G81" t="s" s="481">
+        <v>204</v>
+      </c>
+      <c r="H81" t="s" s="482">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="35">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A23"/>
@@ -5921,6 +6644,7 @@
     <mergeCell ref="A47:A52"/>
     <mergeCell ref="A53:A61"/>
     <mergeCell ref="A62:A74"/>
+    <mergeCell ref="A75:A81"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B23"/>
     <mergeCell ref="B24:B30"/>
@@ -5929,6 +6653,7 @@
     <mergeCell ref="B47:B52"/>
     <mergeCell ref="B53:B61"/>
     <mergeCell ref="B62:B74"/>
+    <mergeCell ref="B75:B81"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -5936,121 +6661,168 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="42.3125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="23.4375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.24609375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="16.99609375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="23.4375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="26.33203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.0078125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="18.91015625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="14.96484375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="15.08984375" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.5625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.3125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.4375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0078125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.24609375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.99609375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.4375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="38.40234375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.91015625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.96484375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="15.08984375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.5625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="420">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s" s="420">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s" s="420">
         <v>92</v>
       </c>
-      <c r="B1" t="s" s="420">
+      <c r="D1" t="s" s="420">
         <v>93</v>
       </c>
-      <c r="C1" t="s" s="420">
+      <c r="E1" t="s" s="420">
         <v>94</v>
       </c>
-      <c r="D1" t="s" s="420">
+      <c r="F1" t="s" s="420">
         <v>95</v>
       </c>
-      <c r="E1" t="s" s="420">
+      <c r="G1" t="s" s="420">
         <v>96</v>
       </c>
-      <c r="F1" t="s" s="420">
+      <c r="H1" t="s" s="420">
         <v>97</v>
       </c>
-      <c r="G1" t="s" s="420">
+      <c r="I1" t="s" s="420">
         <v>98</v>
       </c>
-      <c r="H1" t="s" s="420">
+      <c r="J1" t="s" s="420">
         <v>99</v>
       </c>
-      <c r="I1" t="s" s="420">
+      <c r="K1" t="s" s="420">
         <v>100</v>
       </c>
-      <c r="J1" t="s" s="420">
+      <c r="L1" t="s" s="420">
         <v>101</v>
       </c>
-      <c r="K1" t="s" s="420">
+      <c r="M1" t="s" s="420">
         <v>102</v>
       </c>
-      <c r="L1" t="s" s="420">
+      <c r="N1" t="s" s="420">
         <v>103</v>
       </c>
-      <c r="M1" t="s" s="420">
+      <c r="O1" t="s" s="420">
         <v>104</v>
-      </c>
-      <c r="N1" t="s" s="420">
-        <v>105</v>
-      </c>
-      <c r="O1" t="s" s="420">
-        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="421">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s" s="421">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s" s="421">
         <v>107</v>
       </c>
-      <c r="B2" t="s" s="421">
+      <c r="D2" t="s" s="421">
         <v>108</v>
       </c>
-      <c r="C2" t="s" s="421">
+      <c r="E2" t="s" s="421">
         <v>109</v>
       </c>
-      <c r="D2" t="s" s="421">
+      <c r="F2" t="s" s="421">
         <v>110</v>
       </c>
-      <c r="E2" t="s" s="421">
+      <c r="G2" t="s" s="421">
         <v>111</v>
       </c>
-      <c r="F2" t="s" s="421">
+      <c r="H2" t="s" s="421">
         <v>112</v>
-      </c>
-      <c r="G2" t="s" s="421">
-        <v>113</v>
-      </c>
-      <c r="H2" t="s" s="421">
-        <v>114</v>
       </c>
       <c r="I2" t="n" s="421">
         <v>69.0</v>
       </c>
       <c r="J2" t="n" s="421">
-        <v>68.0</v>
+        <v>69.0</v>
       </c>
       <c r="K2" t="n" s="421">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L2" t="n" s="421">
         <v>0.0</v>
       </c>
       <c r="M2" t="s" s="421">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N2" t="s" s="421">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O2" t="s" s="422">
-        <v>89</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="487">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s" s="487">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s" s="487">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s" s="487">
+        <v>205</v>
+      </c>
+      <c r="E3" t="s" s="487">
+        <v>109</v>
+      </c>
+      <c r="F3" t="s" s="487">
+        <v>110</v>
+      </c>
+      <c r="G3" t="s" s="487">
+        <v>111</v>
+      </c>
+      <c r="H3" t="s" s="487">
+        <v>206</v>
+      </c>
+      <c r="I3" t="n" s="487">
+        <v>7.0</v>
+      </c>
+      <c r="J3" t="n" s="487">
+        <v>7.0</v>
+      </c>
+      <c r="K3" t="n" s="487">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n" s="487">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="s" s="487">
+        <v>113</v>
+      </c>
+      <c r="N3" t="s" s="487">
+        <v>207</v>
+      </c>
+      <c r="O3" t="s" s="488">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -6058,7 +6830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H20"/>
   <sheetViews>
@@ -6077,215 +6849,215 @@
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="true">
-      <c r="A1" t="s" s="424">
+      <c r="A1" t="s" s="490">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" ht="18.0" customHeight="true">
+      <c r="A2" t="s" s="491">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" ht="18.0" customHeight="true">
+      <c r="A4" t="s" s="489">
         <v>117</v>
       </c>
     </row>
-    <row r="2" ht="18.0" customHeight="true">
-      <c r="A2" t="s" s="425">
+    <row r="5" ht="18.0" customHeight="true">
+      <c r="A5" t="s" s="497">
         <v>118</v>
       </c>
-    </row>
-    <row r="4" ht="18.0" customHeight="true">
-      <c r="A4" t="s" s="423">
+      <c r="B5" t="s" s="492">
         <v>119</v>
       </c>
-    </row>
-    <row r="5" ht="18.0" customHeight="true">
-      <c r="A5" t="s" s="431">
+      <c r="D5" t="s" s="497">
         <v>120</v>
       </c>
-      <c r="B5" t="s" s="426">
+      <c r="E5" t="s" s="492">
         <v>121</v>
       </c>
-      <c r="D5" t="s" s="431">
+      <c r="G5" t="s" s="497">
         <v>122</v>
       </c>
-      <c r="E5" t="s" s="426">
+      <c r="H5" t="s" s="492">
         <v>123</v>
       </c>
-      <c r="G5" t="s" s="431">
+    </row>
+    <row r="6" ht="18.0" customHeight="true">
+      <c r="A6" t="s" s="497">
         <v>124</v>
       </c>
-      <c r="H5" t="s" s="426">
+      <c r="B6" t="s" s="492">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s" s="497">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" ht="18.0" customHeight="true">
-      <c r="A6" t="s" s="431">
+      <c r="E6" t="s" s="492">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s" s="497">
         <v>126</v>
       </c>
-      <c r="B6" t="s" s="426">
-        <v>115</v>
-      </c>
-      <c r="D6" t="s" s="431">
+      <c r="H6" t="s" s="496">
         <v>127</v>
       </c>
-      <c r="E6" t="s" s="426">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s" s="431">
+    </row>
+    <row r="8" ht="18.0" customHeight="true">
+      <c r="A8" t="s" s="489">
         <v>128</v>
       </c>
-      <c r="H6" t="s" s="430">
+    </row>
+    <row r="9" ht="18.0" customHeight="true">
+      <c r="A9" t="s" s="497">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" ht="18.0" customHeight="true">
-      <c r="A8" t="s" s="423">
+      <c r="B9" t="s" s="496">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" ht="18.0" customHeight="true">
-      <c r="A9" t="s" s="431">
+      <c r="D9" t="s" s="497">
         <v>131</v>
       </c>
-      <c r="B9" t="s" s="430">
+      <c r="E9" t="s" s="496">
         <v>132</v>
       </c>
-      <c r="D9" t="s" s="431">
+      <c r="G9" t="s" s="497">
         <v>133</v>
       </c>
-      <c r="E9" t="s" s="430">
-        <v>134</v>
-      </c>
-      <c r="G9" t="s" s="431">
+      <c r="H9" t="s" s="495">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" ht="18.0" customHeight="true">
+      <c r="A10" t="s" s="497">
         <v>135</v>
       </c>
-      <c r="H9" t="s" s="429">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" ht="18.0" customHeight="true">
-      <c r="A10" t="s" s="431">
+      <c r="B10" t="s" s="495">
+        <v>210</v>
+      </c>
+      <c r="D10" t="s" s="497">
         <v>137</v>
       </c>
-      <c r="B10" t="s" s="429">
-        <v>138</v>
-      </c>
-      <c r="D10" t="s" s="431">
+      <c r="E10" t="s" s="495">
+        <v>211</v>
+      </c>
+      <c r="G10" t="s" s="497">
         <v>139</v>
       </c>
-      <c r="E10" t="s" s="429">
+      <c r="H10" t="s" s="496">
         <v>140</v>
       </c>
-      <c r="G10" t="s" s="431">
+    </row>
+    <row r="11" ht="18.0" customHeight="true">
+      <c r="A11" t="s" s="497">
         <v>141</v>
       </c>
-      <c r="H10" t="s" s="430">
+      <c r="B11" t="s" s="496">
+        <v>212</v>
+      </c>
+      <c r="D11" t="s" s="497">
         <v>142</v>
       </c>
-    </row>
-    <row r="11" ht="18.0" customHeight="true">
-      <c r="A11" t="s" s="431">
-        <v>143</v>
-      </c>
-      <c r="B11" t="s" s="430">
-        <v>116</v>
-      </c>
-      <c r="D11" t="s" s="431">
+      <c r="E11" t="s" s="495">
+        <v>213</v>
+      </c>
+      <c r="G11" t="s" s="497">
         <v>144</v>
       </c>
-      <c r="E11" t="s" s="429">
-        <v>145</v>
-      </c>
-      <c r="G11" t="s" s="431">
+      <c r="H11" t="s" s="495">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" ht="18.0" customHeight="true">
+      <c r="A13" t="s" s="489">
         <v>146</v>
       </c>
-      <c r="H11" t="s" s="429">
+    </row>
+    <row r="14" ht="18.0" customHeight="true">
+      <c r="A14" t="s" s="497">
         <v>147</v>
       </c>
-    </row>
-    <row r="13" ht="18.0" customHeight="true">
-      <c r="A13" t="s" s="423">
+      <c r="B14" t="s" s="494">
         <v>148</v>
       </c>
-    </row>
-    <row r="14" ht="18.0" customHeight="true">
-      <c r="A14" t="s" s="431">
+      <c r="D14" t="s" s="497">
         <v>149</v>
       </c>
-      <c r="B14" t="s" s="428">
-        <v>150</v>
-      </c>
-      <c r="D14" t="s" s="431">
+      <c r="E14" t="s" s="492">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" ht="18.0" customHeight="true">
+      <c r="A15" t="s" s="497">
         <v>151</v>
       </c>
-      <c r="E14" t="s" s="426">
+      <c r="B15" t="s" s="495">
+        <v>148</v>
+      </c>
+      <c r="D15" t="s" s="497">
         <v>152</v>
       </c>
-    </row>
-    <row r="15" ht="18.0" customHeight="true">
-      <c r="A15" t="s" s="431">
+      <c r="E15" t="s" s="494">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" ht="18.0" customHeight="true">
+      <c r="A16" t="s" s="497">
         <v>153</v>
       </c>
-      <c r="B15" t="s" s="429">
-        <v>150</v>
-      </c>
-      <c r="D15" t="s" s="431">
-        <v>154</v>
-      </c>
-      <c r="E15" t="s" s="428">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" ht="18.0" customHeight="true">
-      <c r="A16" t="s" s="431">
+      <c r="B16" t="s" s="492">
+        <v>216</v>
+      </c>
+      <c r="D16" t="s" s="492">
         <v>155</v>
       </c>
-      <c r="B16" t="s" s="426">
+      <c r="F16" t="s" s="492">
         <v>156</v>
       </c>
-      <c r="D16" t="s" s="428">
+    </row>
+    <row r="18" ht="18.0" customHeight="true">
+      <c r="A18" t="s" s="489">
         <v>157</v>
       </c>
-      <c r="F16" t="s" s="426">
+    </row>
+    <row r="19" ht="18.0" customHeight="true">
+      <c r="A19" t="s" s="497">
         <v>158</v>
       </c>
-    </row>
-    <row r="18" ht="18.0" customHeight="true">
-      <c r="A18" t="s" s="423">
+      <c r="B19" t="s" s="496">
         <v>159</v>
       </c>
-    </row>
-    <row r="19" ht="18.0" customHeight="true">
-      <c r="A19" t="s" s="431">
+      <c r="D19" t="s" s="497">
         <v>160</v>
       </c>
-      <c r="B19" t="s" s="430">
+      <c r="E19" t="s" s="492">
         <v>161</v>
       </c>
-      <c r="D19" t="s" s="431">
+      <c r="G19" t="s" s="497">
         <v>162</v>
       </c>
-      <c r="E19" t="s" s="426">
+      <c r="H19" t="s" s="492">
         <v>163</v>
       </c>
-      <c r="G19" t="s" s="431">
+    </row>
+    <row r="20" ht="18.0" customHeight="true">
+      <c r="A20" t="s" s="497">
         <v>164</v>
       </c>
-      <c r="H19" t="s" s="426">
+      <c r="B20" t="s" s="492">
         <v>165</v>
       </c>
-    </row>
-    <row r="20" ht="18.0" customHeight="true">
-      <c r="A20" t="s" s="431">
+      <c r="D20" t="s" s="497">
         <v>166</v>
       </c>
-      <c r="B20" t="s" s="426">
+      <c r="E20" t="s" s="492">
         <v>167</v>
       </c>
-      <c r="D20" t="s" s="431">
+      <c r="G20" t="s" s="497">
         <v>168</v>
       </c>
-      <c r="E20" t="s" s="426">
+      <c r="H20" t="s" s="493">
         <v>169</v>
-      </c>
-      <c r="G20" t="s" s="431">
-        <v>170</v>
-      </c>
-      <c r="H20" t="s" s="427">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -6301,7 +7073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -6320,207 +7092,207 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="433">
+      <c r="A1" t="s" s="499">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="500">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="498">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="506">
         <v>172</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="434">
+      <c r="B5" t="s" s="504">
         <v>173</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="432">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="440">
+      <c r="D5" t="s" s="506">
         <v>174</v>
       </c>
-      <c r="B5" t="s" s="438">
+      <c r="E5" t="s" s="504">
+        <v>173</v>
+      </c>
+      <c r="G5" t="s" s="506">
+        <v>122</v>
+      </c>
+      <c r="H5" t="s" s="504">
         <v>175</v>
       </c>
-      <c r="D5" t="s" s="440">
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="506">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s" s="504">
         <v>176</v>
       </c>
-      <c r="E5" t="s" s="438">
-        <v>175</v>
-      </c>
-      <c r="G5" t="s" s="440">
-        <v>124</v>
-      </c>
-      <c r="H5" t="s" s="438">
+      <c r="D6" t="s" s="506">
+        <v>125</v>
+      </c>
+      <c r="E6" t="s" s="504">
         <v>177</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="440">
-        <v>122</v>
-      </c>
-      <c r="B6" t="s" s="438">
+      <c r="G6" t="s" s="506">
+        <v>126</v>
+      </c>
+      <c r="H6" t="s" s="501">
         <v>178</v>
       </c>
-      <c r="D6" t="s" s="440">
-        <v>127</v>
-      </c>
-      <c r="E6" t="s" s="438">
-        <v>89</v>
-      </c>
-      <c r="G6" t="s" s="440">
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="498">
         <v>128</v>
       </c>
-      <c r="H6" t="s" s="435">
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="506">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s" s="505">
+        <v>130</v>
+      </c>
+      <c r="D9" t="s" s="506">
+        <v>131</v>
+      </c>
+      <c r="E9" t="s" s="505">
+        <v>132</v>
+      </c>
+      <c r="G9" t="s" s="506">
         <v>179</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="432">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="440">
-        <v>131</v>
-      </c>
-      <c r="B9" t="s" s="439">
-        <v>132</v>
-      </c>
-      <c r="D9" t="s" s="440">
-        <v>133</v>
-      </c>
-      <c r="E9" t="s" s="439">
-        <v>134</v>
-      </c>
-      <c r="G9" t="s" s="440">
+      <c r="H9" t="s" s="505">
         <v>180</v>
       </c>
-      <c r="H9" t="s" s="439">
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="506">
+        <v>135</v>
+      </c>
+      <c r="B10" t="s" s="504">
         <v>181</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="440">
-        <v>137</v>
-      </c>
-      <c r="B10" t="s" s="438">
+      <c r="D10" t="s" s="506">
         <v>182</v>
       </c>
-      <c r="D10" t="s" s="440">
+      <c r="E10" t="s" s="502">
         <v>183</v>
       </c>
-      <c r="E10" t="s" s="436">
+      <c r="G10" t="s" s="506">
+        <v>139</v>
+      </c>
+      <c r="H10" t="s" s="505">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="506">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s" s="505">
+        <v>180</v>
+      </c>
+      <c r="D11" t="s" s="506">
         <v>184</v>
       </c>
-      <c r="G10" t="s" s="440">
-        <v>141</v>
-      </c>
-      <c r="H10" t="s" s="439">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="440">
-        <v>143</v>
-      </c>
-      <c r="B11" t="s" s="439">
-        <v>181</v>
-      </c>
-      <c r="D11" t="s" s="440">
+      <c r="E11" t="s" s="501">
         <v>185</v>
       </c>
-      <c r="E11" t="s" s="435">
+      <c r="G11" t="s" s="506">
         <v>186</v>
       </c>
-      <c r="G11" t="s" s="440">
+      <c r="H11" t="s" s="504">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="498">
         <v>187</v>
       </c>
-      <c r="H11" t="s" s="438">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="432">
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="506">
         <v>188</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="440">
+      <c r="B14" t="s" s="505">
         <v>189</v>
       </c>
-      <c r="B14" t="s" s="439">
+      <c r="D14" t="s" s="506">
         <v>190</v>
       </c>
-      <c r="D14" t="s" s="440">
+      <c r="E14" t="s" s="505">
+        <v>189</v>
+      </c>
+      <c r="G14" t="s" s="506">
         <v>191</v>
       </c>
-      <c r="E14" t="s" s="439">
-        <v>190</v>
-      </c>
-      <c r="G14" t="s" s="440">
+      <c r="H14" t="s" s="505">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="506">
+        <v>153</v>
+      </c>
+      <c r="B15" t="s" s="501">
         <v>192</v>
       </c>
-      <c r="H14" t="s" s="439">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="440">
+      <c r="D15" t="s" s="501">
         <v>155</v>
       </c>
-      <c r="B15" t="s" s="435">
+      <c r="F15" t="s" s="501">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="498">
         <v>193</v>
       </c>
-      <c r="D15" t="s" s="435">
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="506">
         <v>194</v>
       </c>
-      <c r="F15" t="s" s="435">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="432">
+      <c r="B18" t="s" s="501">
         <v>195</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="440">
+      <c r="D18" t="s" s="506">
+        <v>160</v>
+      </c>
+      <c r="E18" t="s" s="501">
+        <v>165</v>
+      </c>
+      <c r="G18" t="s" s="506">
+        <v>162</v>
+      </c>
+      <c r="H18" t="s" s="502">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="506">
         <v>196</v>
       </c>
-      <c r="B18" t="s" s="435">
+      <c r="B19" t="s" s="501">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s" s="506">
+        <v>166</v>
+      </c>
+      <c r="E19" t="s" s="502">
         <v>197</v>
       </c>
-      <c r="D18" t="s" s="440">
-        <v>162</v>
-      </c>
-      <c r="E18" t="s" s="435">
-        <v>167</v>
-      </c>
-      <c r="G18" t="s" s="440">
-        <v>164</v>
-      </c>
-      <c r="H18" t="s" s="436">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="440">
+      <c r="G19" t="s" s="506">
+        <v>168</v>
+      </c>
+      <c r="H19" t="s" s="502">
         <v>198</v>
-      </c>
-      <c r="B19" t="s" s="435">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s" s="440">
-        <v>168</v>
-      </c>
-      <c r="E19" t="s" s="436">
-        <v>199</v>
-      </c>
-      <c r="G19" t="s" s="440">
-        <v>170</v>
-      </c>
-      <c r="H19" t="s" s="436">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Performance fix: Replace slow checkbox iteration with JavaScript counting in PO42
- verify_loaded_profiles_are_unselected: Use countAllProfilesJS + countSelectedProfilesJS
- verify_all_loaded_profiles_are_unselected: Use JavaScript counting instead of loop
- verify_profiles_loaded_after_header_checkbox_are_not_selected: Use JavaScript counting
- Speedup: From 10+ minutes to <1 second for verification steps with 8000+ profiles
- Cleanup: Remove old backup files and template
</commit_message>
<xml_diff>
--- a/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
+++ b/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
@@ -6,16 +6,16 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Results Summary" r:id="rId3" sheetId="1"/>
     <sheet name="Automation Execution History" r:id="rId4" sheetId="2"/>
-    <sheet name="Automation QA Dashboard" r:id="rId6" sheetId="7"/>
-    <sheet name="Cross-Browser QA Dashboard" r:id="rId7" sheetId="8"/>
+    <sheet name="Test Results Summary" r:id="rId8" sheetId="9"/>
+    <sheet name="Automation QA Dashboard" r:id="rId9" sheetId="10"/>
+    <sheet name="Cross-Browser QA Dashboard" r:id="rId10" sheetId="11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="231">
   <si>
     <t>Test Results Summary - 2025-12-18 18:56:37</t>
   </si>
@@ -660,13 +660,98 @@
   <si>
     <t>Generated: 2025-12-18 19:54:16 | Environment: qa | Focus: Cross-Browser Multi-Platform Execution</t>
   </si>
+  <si>
+    <t>Test Results Summary - 2025-12-19 09:30:41</t>
+  </si>
+  <si>
+    <t>Daily Status [2025-12-19]: FAILED (1 run)</t>
+  </si>
+  <si>
+    <t>Total: 16</t>
+  </si>
+  <si>
+    <t>Passed: 15</t>
+  </si>
+  <si>
+    <t>Failed: 1</t>
+  </si>
+  <si>
+    <t>Duration: 13m 22s</t>
+  </si>
+  <si>
+    <t>Time: 09:30:41 | Total: 16 | Pass: 15 | Fail: 1</t>
+  </si>
+  <si>
+    <t>Exception: AssertionError
+Message: Publish Selected Profiles button should be disabled but is enabled
+Key Stack Trace:
+  at org.testng.Assert.fail(Assert.java:111)
+  at com.kfonetalentsuite.pageobjects.JobMapping.PO42_ClearProfileSelectionFunctionality.verify_action_button_is_disabled(PO42_ClearProfileSelectionFunctionality.java:547)</t>
+  </si>
+  <si>
+    <t>2025-12-19</t>
+  </si>
+  <si>
+    <t>09:30:41</t>
+  </si>
+  <si>
+    <t>94.0%</t>
+  </si>
+  <si>
+    <t>13m 22s</t>
+  </si>
+  <si>
+    <t>Generated: 2025-12-19 09:30:41 | Environment: qa | Focus: Normal Single-Browser Execution</t>
+  </si>
+  <si>
+    <t>94%</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>298</t>
+  </si>
+  <si>
+    <t>50.1s</t>
+  </si>
+  <si>
+    <t>1 of 44 (2.3%)</t>
+  </si>
+  <si>
+    <t>16 of 298 (5.4%)</t>
+  </si>
+  <si>
+    <t>5.4%</t>
+  </si>
+  <si>
+    <t>2.3%</t>
+  </si>
+  <si>
+    <t>16 scenarios</t>
+  </si>
+  <si>
+    <t>15 Passed</t>
+  </si>
+  <si>
+    <t>1 Failed</t>
+  </si>
+  <si>
+    <t>Generated: 2025-12-19 09:30:41 | Environment: qa | Focus: Cross-Browser Multi-Platform Execution</t>
+  </si>
+  <si>
+    <t>0 of 44 (0.0%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="311">
+  <fonts count="428">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -2108,6 +2193,542 @@
       <sz val="10.0"/>
       <b val="true"/>
       <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -2388,7 +3009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="323">
+  <cellXfs count="444">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
@@ -3354,634 +3975,848 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="310" fillId="21" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="311" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="312" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="313" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="314" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="315" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="316" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="317" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="318" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="319" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="320" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="321" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="322" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="323" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="324" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="325" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="326" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="327" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="328" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="329" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="330" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="331" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="332" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="333" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="334" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="335" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="336" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="337" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="338" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="339" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="340" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="341" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="342" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="343" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="344" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="345" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="346" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="347" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="348" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="349" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="350" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="351" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="352" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="353" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="354" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="355" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="356" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="357" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="358" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="359" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="360" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="361" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="362" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="363" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="364" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="365" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="366" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="367" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="368" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="369" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="370" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="371" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="372" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="373" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="374" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="375" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="376" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="377" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="378" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="379" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="380" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="381" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="382" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="383" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="384" fillId="7" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="385" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="386" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="387" fillId="7" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="388" fillId="7" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="389" fillId="7" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="390" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="391" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="392" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="393" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="394" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="395" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="396" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="397" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="398" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="399" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="400" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="401" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="402" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="403" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="404" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="405" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="406" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="407" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="408" fillId="7" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="409" fillId="7" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="410" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="411" fillId="11" borderId="10" xfId="0" applyFont="true" applyFill="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="412" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="413" fillId="15" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="414" fillId="5" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="415" fillId="17" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="416" fillId="19" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="417" fillId="9" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="418" fillId="21" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="419" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="420" fillId="11" borderId="10" xfId="0" applyFont="true" applyFill="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="421" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="422" fillId="15" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="423" fillId="5" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="424" fillId="17" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="425" fillId="19" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="426" fillId="9" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="427" fillId="21" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="39.0625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="48.86328125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="67.80859375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.71875"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.71875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.7734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.10546875"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="255.0"/>
+    <col min="1" max="1" width="21.46875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.84375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="22.19140625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.84375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.671875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="17.546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.84375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.671875" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.0" customHeight="true">
+      <c r="A1" t="s" s="427">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" ht="18.0" customHeight="true">
+      <c r="A2" t="s" s="428">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" ht="18.0" customHeight="true">
+      <c r="A4" t="s" s="426">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" ht="18.0" customHeight="true">
+      <c r="A5" t="s" s="434">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s" s="429">
+        <v>217</v>
+      </c>
+      <c r="D5" t="s" s="434">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s" s="431">
+        <v>218</v>
+      </c>
+      <c r="G5" t="s" s="434">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s" s="431">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" ht="18.0" customHeight="true">
+      <c r="A6" t="s" s="434">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s" s="429">
+        <v>214</v>
+      </c>
+      <c r="D6" t="s" s="434">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s" s="432">
+        <v>111</v>
+      </c>
+      <c r="G6" t="s" s="434">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s" s="433">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" ht="18.0" customHeight="true">
+      <c r="A8" t="s" s="426">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" ht="18.0" customHeight="true">
+      <c r="A9" t="s" s="434">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s" s="433">
+        <v>219</v>
+      </c>
+      <c r="D9" t="s" s="434">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s" s="433">
+        <v>220</v>
+      </c>
+      <c r="G9" t="s" s="434">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s" s="432">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" ht="18.0" customHeight="true">
+      <c r="A10" t="s" s="434">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s" s="432">
+        <v>222</v>
+      </c>
+      <c r="D10" t="s" s="434">
+        <v>71</v>
+      </c>
+      <c r="E10" t="s" s="432">
+        <v>223</v>
+      </c>
+      <c r="G10" t="s" s="434">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s" s="433">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" ht="18.0" customHeight="true">
+      <c r="A11" t="s" s="434">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s" s="433">
+        <v>215</v>
+      </c>
+      <c r="D11" t="s" s="434">
+        <v>76</v>
+      </c>
+      <c r="E11" t="s" s="432">
+        <v>224</v>
+      </c>
+      <c r="G11" t="s" s="434">
+        <v>78</v>
+      </c>
+      <c r="H11" t="s" s="432">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" ht="18.0" customHeight="true">
+      <c r="A13" t="s" s="426">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" ht="18.0" customHeight="true">
+      <c r="A14" t="s" s="434">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s" s="431">
+        <v>82</v>
+      </c>
+      <c r="D14" t="s" s="434">
+        <v>83</v>
+      </c>
+      <c r="E14" t="s" s="432">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" ht="18.0" customHeight="true">
+      <c r="A15" t="s" s="434">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s" s="429">
+        <v>226</v>
+      </c>
+      <c r="D15" t="s" s="434">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s" s="431">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" ht="18.0" customHeight="true">
+      <c r="A16" t="s" s="434">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s" s="429">
+        <v>227</v>
+      </c>
+      <c r="D16" t="s" s="431">
+        <v>228</v>
+      </c>
+      <c r="F16" t="s" s="429">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" ht="18.0" customHeight="true">
+      <c r="A18" t="s" s="426">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" ht="18.0" customHeight="true">
+      <c r="A19" t="s" s="434">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s" s="433">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s" s="434">
+        <v>94</v>
+      </c>
+      <c r="E19" t="s" s="429">
+        <v>95</v>
+      </c>
+      <c r="G19" t="s" s="434">
+        <v>96</v>
+      </c>
+      <c r="H19" t="s" s="429">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" ht="18.0" customHeight="true">
+      <c r="A20" t="s" s="434">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s" s="429">
+        <v>99</v>
+      </c>
+      <c r="D20" t="s" s="434">
+        <v>100</v>
+      </c>
+      <c r="E20" t="s" s="429">
+        <v>101</v>
+      </c>
+      <c r="G20" t="s" s="434">
+        <v>102</v>
+      </c>
+      <c r="H20" t="s" s="430">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A18:H18"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="19.53125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.71875" customWidth="true"/>
+    <col min="4" max="4" width="19.53125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="17.578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.71875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="17.578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="17.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>161</v>
+      <c r="A1" t="s" s="436">
+        <v>104</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>162</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>163</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>164</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>165</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>166</v>
+    <row r="2">
+      <c r="A2" t="s" s="437">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="435">
+        <v>51</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="1">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s" s="1">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s" s="1">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s" s="1">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s" s="1">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s" s="1">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s" s="1">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s" s="1">
-        <v>14</v>
+      <c r="A5" t="s" s="443">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s" s="441">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s" s="443">
+        <v>108</v>
+      </c>
+      <c r="E5" t="s" s="441">
+        <v>107</v>
+      </c>
+      <c r="G5" t="s" s="443">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s" s="441">
+        <v>109</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="216">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s" s="218">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s" s="219">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s" s="220">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s" s="221">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s" s="222">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s" s="219">
-        <v>138</v>
-      </c>
-      <c r="H6" t="s" s="219">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="216">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s" s="218">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s" s="223">
-        <v>139</v>
-      </c>
-      <c r="D7" t="s" s="224">
+      <c r="A6" t="s" s="443">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s" s="441">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s" s="443">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s" s="441">
         <v>111</v>
       </c>
-      <c r="E7" t="s" s="225">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s" s="226">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s" s="223">
-        <v>138</v>
-      </c>
-      <c r="H7" t="s" s="223">
-        <v>140</v>
+      <c r="G6" t="s" s="443">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s" s="438">
+        <v>112</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="216">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s" s="218">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s" s="227">
-        <v>141</v>
-      </c>
-      <c r="D8" t="s" s="228">
-        <v>111</v>
-      </c>
-      <c r="E8" t="s" s="229">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s" s="230">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s" s="227">
-        <v>138</v>
-      </c>
-      <c r="H8" t="s" s="227">
-        <v>142</v>
+      <c r="A8" t="s" s="435">
+        <v>62</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="216">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s" s="218">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s" s="231">
-        <v>143</v>
-      </c>
-      <c r="D9" t="s" s="232">
-        <v>111</v>
-      </c>
-      <c r="E9" t="s" s="233">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s" s="234">
-        <v>19</v>
-      </c>
-      <c r="G9" t="s" s="231">
-        <v>138</v>
-      </c>
-      <c r="H9" t="s" s="231">
-        <v>144</v>
+      <c r="A9" t="s" s="443">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s" s="442">
+        <v>219</v>
+      </c>
+      <c r="D9" t="s" s="443">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s" s="442">
+        <v>220</v>
+      </c>
+      <c r="G9" t="s" s="443">
+        <v>113</v>
+      </c>
+      <c r="H9" t="s" s="442">
+        <v>114</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="216">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s" s="218">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s" s="235">
-        <v>145</v>
-      </c>
-      <c r="D10" t="s" s="236">
-        <v>111</v>
-      </c>
-      <c r="E10" t="s" s="237">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s" s="238">
-        <v>19</v>
-      </c>
-      <c r="G10" t="s" s="235">
-        <v>138</v>
-      </c>
-      <c r="H10" t="s" s="235">
-        <v>142</v>
+      <c r="A10" t="s" s="443">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s" s="441">
+        <v>230</v>
+      </c>
+      <c r="D10" t="s" s="443">
+        <v>116</v>
+      </c>
+      <c r="E10" t="s" s="439">
+        <v>117</v>
+      </c>
+      <c r="G10" t="s" s="443">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s" s="442">
+        <v>43</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B11" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C11" t="s" s="239">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s" s="240">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s" s="241">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s" s="242">
-        <v>19</v>
-      </c>
-      <c r="G11" t="s" s="239">
-        <v>169</v>
-      </c>
-      <c r="H11" t="s" s="239">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B12" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C12" t="s" s="243">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s" s="244">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s" s="245">
-        <v>19</v>
-      </c>
-      <c r="F12" t="s" s="246">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s" s="243">
-        <v>169</v>
-      </c>
-      <c r="H12" t="s" s="243">
-        <v>21</v>
+      <c r="A11" t="s" s="443">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s" s="442">
+        <v>114</v>
+      </c>
+      <c r="D11" t="s" s="443">
+        <v>118</v>
+      </c>
+      <c r="E11" t="s" s="438">
+        <v>119</v>
+      </c>
+      <c r="G11" t="s" s="443">
+        <v>120</v>
+      </c>
+      <c r="H11" t="s" s="441">
+        <v>107</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B13" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C13" t="s" s="247">
-        <v>170</v>
-      </c>
-      <c r="D13" t="s" s="248">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s" s="249">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s" s="250">
-        <v>19</v>
-      </c>
-      <c r="G13" t="s" s="247">
-        <v>169</v>
-      </c>
-      <c r="H13" t="s" s="247">
-        <v>21</v>
+      <c r="A13" t="s" s="435">
+        <v>121</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B14" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C14" t="s" s="251">
-        <v>171</v>
-      </c>
-      <c r="D14" t="s" s="252">
-        <v>111</v>
-      </c>
-      <c r="E14" t="s" s="253">
-        <v>19</v>
-      </c>
-      <c r="F14" t="s" s="254">
-        <v>19</v>
-      </c>
-      <c r="G14" t="s" s="251">
-        <v>169</v>
-      </c>
-      <c r="H14" t="s" s="251">
-        <v>172</v>
+      <c r="A14" t="s" s="443">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s" s="442">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s" s="443">
+        <v>124</v>
+      </c>
+      <c r="E14" t="s" s="442">
+        <v>123</v>
+      </c>
+      <c r="G14" t="s" s="443">
+        <v>125</v>
+      </c>
+      <c r="H14" t="s" s="442">
+        <v>123</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B15" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C15" t="s" s="255">
-        <v>173</v>
-      </c>
-      <c r="D15" t="s" s="256">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s" s="257">
-        <v>19</v>
-      </c>
-      <c r="F15" t="s" s="258">
-        <v>19</v>
-      </c>
-      <c r="G15" t="s" s="255">
-        <v>169</v>
-      </c>
-      <c r="H15" t="s" s="255">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B16" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C16" t="s" s="259">
-        <v>174</v>
-      </c>
-      <c r="D16" t="s" s="260">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s" s="261">
-        <v>19</v>
-      </c>
-      <c r="F16" t="s" s="262">
-        <v>19</v>
-      </c>
-      <c r="G16" t="s" s="259">
-        <v>169</v>
-      </c>
-      <c r="H16" t="s" s="259">
-        <v>21</v>
+      <c r="A15" t="s" s="443">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s" s="438">
+        <v>126</v>
+      </c>
+      <c r="D15" t="s" s="438">
+        <v>89</v>
+      </c>
+      <c r="F15" t="s" s="438">
+        <v>90</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B17" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C17" t="s" s="263">
-        <v>175</v>
-      </c>
-      <c r="D17" t="s" s="264">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s" s="265">
-        <v>19</v>
-      </c>
-      <c r="F17" t="s" s="266">
-        <v>19</v>
-      </c>
-      <c r="G17" t="s" s="263">
-        <v>169</v>
-      </c>
-      <c r="H17" t="s" s="263">
-        <v>21</v>
+      <c r="A17" t="s" s="435">
+        <v>127</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B18" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C18" t="s" s="267">
-        <v>176</v>
-      </c>
-      <c r="D18" t="s" s="268">
-        <v>18</v>
-      </c>
-      <c r="E18" t="s" s="269">
-        <v>19</v>
-      </c>
-      <c r="F18" t="s" s="270">
-        <v>19</v>
-      </c>
-      <c r="G18" t="s" s="267">
-        <v>169</v>
-      </c>
-      <c r="H18" t="s" s="267">
-        <v>21</v>
+      <c r="A18" t="s" s="443">
+        <v>128</v>
+      </c>
+      <c r="B18" t="s" s="438">
+        <v>129</v>
+      </c>
+      <c r="D18" t="s" s="443">
+        <v>94</v>
+      </c>
+      <c r="E18" t="s" s="438">
+        <v>99</v>
+      </c>
+      <c r="G18" t="s" s="443">
+        <v>96</v>
+      </c>
+      <c r="H18" t="s" s="439">
+        <v>97</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B19" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C19" t="s" s="271">
-        <v>177</v>
-      </c>
-      <c r="D19" t="s" s="272">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s" s="273">
-        <v>19</v>
-      </c>
-      <c r="F19" t="s" s="274">
-        <v>19</v>
-      </c>
-      <c r="G19" t="s" s="271">
-        <v>169</v>
-      </c>
-      <c r="H19" t="s" s="271">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B20" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C20" t="s" s="275">
-        <v>178</v>
-      </c>
-      <c r="D20" t="s" s="276">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s" s="277">
-        <v>19</v>
-      </c>
-      <c r="F20" t="s" s="278">
-        <v>19</v>
-      </c>
-      <c r="G20" t="s" s="275">
-        <v>169</v>
-      </c>
-      <c r="H20" t="s" s="275">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B21" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C21" t="s" s="279">
-        <v>179</v>
-      </c>
-      <c r="D21" t="s" s="280">
-        <v>18</v>
-      </c>
-      <c r="E21" t="s" s="281">
-        <v>19</v>
-      </c>
-      <c r="F21" t="s" s="282">
-        <v>19</v>
-      </c>
-      <c r="G21" t="s" s="279">
-        <v>169</v>
-      </c>
-      <c r="H21" t="s" s="279">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B22" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C22" t="s" s="283">
-        <v>180</v>
-      </c>
-      <c r="D22" t="s" s="284">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s" s="285">
-        <v>19</v>
-      </c>
-      <c r="F22" t="s" s="286">
-        <v>19</v>
-      </c>
-      <c r="G22" t="s" s="283">
-        <v>169</v>
-      </c>
-      <c r="H22" t="s" s="283">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B23" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C23" t="s" s="287">
-        <v>181</v>
-      </c>
-      <c r="D23" t="s" s="288">
-        <v>111</v>
-      </c>
-      <c r="E23" t="s" s="289">
-        <v>19</v>
-      </c>
-      <c r="F23" t="s" s="290">
-        <v>19</v>
-      </c>
-      <c r="G23" t="s" s="287">
-        <v>169</v>
-      </c>
-      <c r="H23" t="s" s="287">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B24" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C24" t="s" s="291">
-        <v>183</v>
-      </c>
-      <c r="D24" t="s" s="292">
-        <v>18</v>
-      </c>
-      <c r="E24" t="s" s="293">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s" s="294">
-        <v>19</v>
-      </c>
-      <c r="G24" t="s" s="291">
-        <v>169</v>
-      </c>
-      <c r="H24" t="s" s="291">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B25" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C25" t="s" s="295">
-        <v>184</v>
-      </c>
-      <c r="D25" t="s" s="296">
-        <v>18</v>
-      </c>
-      <c r="E25" t="s" s="297">
-        <v>19</v>
-      </c>
-      <c r="F25" t="s" s="298">
-        <v>19</v>
-      </c>
-      <c r="G25" t="s" s="295">
-        <v>169</v>
-      </c>
-      <c r="H25" t="s" s="295">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="216">
-        <v>167</v>
-      </c>
-      <c r="B26" t="s" s="218">
-        <v>168</v>
-      </c>
-      <c r="C26" t="s" s="299">
-        <v>185</v>
-      </c>
-      <c r="D26" t="s" s="300">
-        <v>18</v>
-      </c>
-      <c r="E26" t="s" s="301">
-        <v>19</v>
-      </c>
-      <c r="F26" t="s" s="302">
-        <v>19</v>
-      </c>
-      <c r="G26" t="s" s="299">
-        <v>169</v>
-      </c>
-      <c r="H26" t="s" s="299">
-        <v>21</v>
+      <c r="A19" t="s" s="443">
+        <v>130</v>
+      </c>
+      <c r="B19" t="s" s="438">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s" s="443">
+        <v>100</v>
+      </c>
+      <c r="E19" t="s" s="439">
+        <v>131</v>
+      </c>
+      <c r="G19" t="s" s="443">
+        <v>102</v>
+      </c>
+      <c r="H19" t="s" s="439">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A26"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B26"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A17:H17"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3989,7 +4824,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4200,484 +5035,548 @@
         <v>111</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="424">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s" s="424">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s" s="424">
+        <v>212</v>
+      </c>
+      <c r="D5" t="s" s="424">
+        <v>213</v>
+      </c>
+      <c r="E5" t="s" s="424">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s" s="424">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s" s="424">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s" s="424">
+        <v>187</v>
+      </c>
+      <c r="I5" t="n" s="424">
+        <v>16.0</v>
+      </c>
+      <c r="J5" t="n" s="424">
+        <v>15.0</v>
+      </c>
+      <c r="K5" t="n" s="424">
+        <v>1.0</v>
+      </c>
+      <c r="L5" t="n" s="424">
+        <v>0.0</v>
+      </c>
+      <c r="M5" t="s" s="424">
+        <v>214</v>
+      </c>
+      <c r="N5" t="s" s="424">
+        <v>215</v>
+      </c>
+      <c r="O5" t="s" s="425">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.46875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="14.84375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="22.19140625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.84375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.671875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="17.546875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.84375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.671875" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18.0" customHeight="true">
-      <c r="A1" t="s" s="306">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" ht="18.0" customHeight="true">
-      <c r="A2" t="s" s="307">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" ht="18.0" customHeight="true">
-      <c r="A4" t="s" s="305">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" ht="18.0" customHeight="true">
-      <c r="A5" t="s" s="313">
-        <v>52</v>
-      </c>
-      <c r="B5" t="s" s="310">
-        <v>191</v>
-      </c>
-      <c r="D5" t="s" s="313">
-        <v>54</v>
-      </c>
-      <c r="E5" t="s" s="311">
-        <v>110</v>
-      </c>
-      <c r="G5" t="s" s="313">
-        <v>56</v>
-      </c>
-      <c r="H5" t="s" s="310">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" ht="18.0" customHeight="true">
-      <c r="A6" t="s" s="313">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s" s="310">
-        <v>193</v>
-      </c>
-      <c r="D6" t="s" s="313">
-        <v>59</v>
-      </c>
-      <c r="E6" t="s" s="311">
-        <v>111</v>
-      </c>
-      <c r="G6" t="s" s="313">
-        <v>60</v>
-      </c>
-      <c r="H6" t="s" s="312">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" ht="18.0" customHeight="true">
-      <c r="A8" t="s" s="305">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" ht="18.0" customHeight="true">
-      <c r="A9" t="s" s="313">
-        <v>63</v>
-      </c>
-      <c r="B9" t="s" s="312">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s" s="313">
-        <v>65</v>
-      </c>
-      <c r="E9" t="s" s="312">
-        <v>66</v>
-      </c>
-      <c r="G9" t="s" s="313">
-        <v>67</v>
-      </c>
-      <c r="H9" t="s" s="311">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" ht="18.0" customHeight="true">
-      <c r="A10" t="s" s="313">
-        <v>69</v>
-      </c>
-      <c r="B10" t="s" s="311">
-        <v>195</v>
-      </c>
-      <c r="D10" t="s" s="313">
-        <v>71</v>
-      </c>
-      <c r="E10" t="s" s="311">
-        <v>196</v>
-      </c>
-      <c r="G10" t="s" s="313">
-        <v>73</v>
-      </c>
-      <c r="H10" t="s" s="312">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" ht="18.0" customHeight="true">
-      <c r="A11" t="s" s="313">
-        <v>75</v>
-      </c>
-      <c r="B11" t="s" s="312">
-        <v>197</v>
-      </c>
-      <c r="D11" t="s" s="313">
-        <v>76</v>
-      </c>
-      <c r="E11" t="s" s="311">
-        <v>198</v>
-      </c>
-      <c r="G11" t="s" s="313">
-        <v>78</v>
-      </c>
-      <c r="H11" t="s" s="311">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" ht="18.0" customHeight="true">
-      <c r="A13" t="s" s="305">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" ht="18.0" customHeight="true">
-      <c r="A14" t="s" s="313">
-        <v>81</v>
-      </c>
-      <c r="B14" t="s" s="310">
-        <v>82</v>
-      </c>
-      <c r="D14" t="s" s="313">
-        <v>83</v>
-      </c>
-      <c r="E14" t="s" s="311">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" ht="18.0" customHeight="true">
-      <c r="A15" t="s" s="313">
-        <v>84</v>
-      </c>
-      <c r="B15" t="s" s="308">
-        <v>200</v>
-      </c>
-      <c r="D15" t="s" s="313">
-        <v>86</v>
-      </c>
-      <c r="E15" t="s" s="310">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" ht="18.0" customHeight="true">
-      <c r="A16" t="s" s="313">
-        <v>87</v>
-      </c>
-      <c r="B16" t="s" s="308">
-        <v>201</v>
-      </c>
-      <c r="D16" t="s" s="311">
-        <v>202</v>
-      </c>
-      <c r="F16" t="s" s="308">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" ht="18.0" customHeight="true">
-      <c r="A18" t="s" s="305">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" ht="18.0" customHeight="true">
-      <c r="A19" t="s" s="313">
-        <v>92</v>
-      </c>
-      <c r="B19" t="s" s="312">
-        <v>93</v>
-      </c>
-      <c r="D19" t="s" s="313">
-        <v>94</v>
-      </c>
-      <c r="E19" t="s" s="308">
-        <v>95</v>
-      </c>
-      <c r="G19" t="s" s="313">
-        <v>96</v>
-      </c>
-      <c r="H19" t="s" s="308">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" ht="18.0" customHeight="true">
-      <c r="A20" t="s" s="313">
-        <v>98</v>
-      </c>
-      <c r="B20" t="s" s="308">
-        <v>99</v>
-      </c>
-      <c r="D20" t="s" s="313">
-        <v>100</v>
-      </c>
-      <c r="E20" t="s" s="308">
-        <v>101</v>
-      </c>
-      <c r="G20" t="s" s="313">
-        <v>102</v>
-      </c>
-      <c r="H20" t="s" s="309">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A18:H18"/>
-  </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="19.53125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="17.578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.71875" customWidth="true"/>
-    <col min="4" max="4" width="19.53125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="17.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="17.578125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="17.578125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="39.0625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="48.86328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="67.80859375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.71875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.71875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="15.7734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="36.10546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="141.09765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="315">
-        <v>104</v>
+      <c r="A1" t="s" s="323">
+        <v>204</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="316">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="314">
-        <v>51</v>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>207</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>208</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>209</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="322">
-        <v>106</v>
-      </c>
-      <c r="B5" t="s" s="320">
-        <v>107</v>
-      </c>
-      <c r="D5" t="s" s="322">
-        <v>108</v>
-      </c>
-      <c r="E5" t="s" s="320">
-        <v>107</v>
-      </c>
-      <c r="G5" t="s" s="322">
-        <v>56</v>
-      </c>
-      <c r="H5" t="s" s="320">
-        <v>109</v>
+      <c r="A5" t="s" s="323">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s" s="323">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="323">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s" s="323">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s" s="323">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s" s="323">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s" s="323">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s" s="323">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="322">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s" s="320">
-        <v>110</v>
-      </c>
-      <c r="D6" t="s" s="322">
-        <v>59</v>
-      </c>
-      <c r="E6" t="s" s="320">
-        <v>111</v>
-      </c>
-      <c r="G6" t="s" s="322">
-        <v>60</v>
-      </c>
-      <c r="H6" t="s" s="317">
-        <v>112</v>
+      <c r="A6" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B6" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C6" t="s" s="327">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s" s="324">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s" s="325">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s" s="326">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s" s="328">
+        <v>210</v>
+      </c>
+      <c r="H6" t="s" s="329">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B7" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C7" t="s" s="333">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s" s="330">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s" s="331">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s" s="332">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s" s="334">
+        <v>210</v>
+      </c>
+      <c r="H7" t="s" s="335">
+        <v>21</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="314">
-        <v>62</v>
+      <c r="A8" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B8" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C8" t="s" s="339">
+        <v>170</v>
+      </c>
+      <c r="D8" t="s" s="336">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s" s="337">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s" s="338">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s" s="340">
+        <v>210</v>
+      </c>
+      <c r="H8" t="s" s="341">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="322">
-        <v>63</v>
-      </c>
-      <c r="B9" t="s" s="321">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s" s="322">
-        <v>65</v>
-      </c>
-      <c r="E9" t="s" s="321">
-        <v>66</v>
-      </c>
-      <c r="G9" t="s" s="322">
-        <v>113</v>
-      </c>
-      <c r="H9" t="s" s="321">
-        <v>114</v>
+      <c r="A9" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B9" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C9" t="s" s="345">
+        <v>171</v>
+      </c>
+      <c r="D9" t="s" s="342">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s" s="343">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s" s="344">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s" s="346">
+        <v>210</v>
+      </c>
+      <c r="H9" t="s" s="347">
+        <v>21</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="322">
-        <v>69</v>
-      </c>
-      <c r="B10" t="s" s="320">
-        <v>115</v>
-      </c>
-      <c r="D10" t="s" s="322">
-        <v>116</v>
-      </c>
-      <c r="E10" t="s" s="318">
-        <v>117</v>
-      </c>
-      <c r="G10" t="s" s="322">
-        <v>73</v>
-      </c>
-      <c r="H10" t="s" s="321">
-        <v>43</v>
+      <c r="A10" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B10" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C10" t="s" s="351">
+        <v>173</v>
+      </c>
+      <c r="D10" t="s" s="348">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s" s="349">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s" s="350">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s" s="352">
+        <v>210</v>
+      </c>
+      <c r="H10" t="s" s="353">
+        <v>21</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="322">
-        <v>75</v>
-      </c>
-      <c r="B11" t="s" s="321">
-        <v>114</v>
-      </c>
-      <c r="D11" t="s" s="322">
-        <v>118</v>
-      </c>
-      <c r="E11" t="s" s="317">
-        <v>119</v>
-      </c>
-      <c r="G11" t="s" s="322">
-        <v>120</v>
-      </c>
-      <c r="H11" t="s" s="320">
-        <v>107</v>
+      <c r="A11" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C11" t="s" s="357">
+        <v>174</v>
+      </c>
+      <c r="D11" t="s" s="354">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s" s="355">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s" s="356">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s" s="358">
+        <v>210</v>
+      </c>
+      <c r="H11" t="s" s="359">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B12" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C12" t="s" s="363">
+        <v>175</v>
+      </c>
+      <c r="D12" t="s" s="360">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s" s="361">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s" s="362">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s" s="364">
+        <v>210</v>
+      </c>
+      <c r="H12" t="s" s="365">
+        <v>21</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="314">
-        <v>121</v>
+      <c r="A13" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B13" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C13" t="s" s="369">
+        <v>176</v>
+      </c>
+      <c r="D13" t="s" s="366">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s" s="367">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s" s="368">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s" s="370">
+        <v>210</v>
+      </c>
+      <c r="H13" t="s" s="371">
+        <v>21</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="322">
-        <v>122</v>
-      </c>
-      <c r="B14" t="s" s="321">
-        <v>123</v>
-      </c>
-      <c r="D14" t="s" s="322">
-        <v>124</v>
-      </c>
-      <c r="E14" t="s" s="321">
-        <v>123</v>
-      </c>
-      <c r="G14" t="s" s="322">
-        <v>125</v>
-      </c>
-      <c r="H14" t="s" s="321">
-        <v>123</v>
+      <c r="A14" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B14" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C14" t="s" s="375">
+        <v>177</v>
+      </c>
+      <c r="D14" t="s" s="372">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s" s="373">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s" s="374">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s" s="376">
+        <v>210</v>
+      </c>
+      <c r="H14" t="s" s="377">
+        <v>21</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="322">
-        <v>87</v>
-      </c>
-      <c r="B15" t="s" s="317">
-        <v>126</v>
-      </c>
-      <c r="D15" t="s" s="317">
-        <v>89</v>
-      </c>
-      <c r="F15" t="s" s="317">
-        <v>90</v>
+      <c r="A15" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B15" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C15" t="s" s="381">
+        <v>178</v>
+      </c>
+      <c r="D15" t="s" s="378">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s" s="379">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s" s="380">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s" s="382">
+        <v>210</v>
+      </c>
+      <c r="H15" t="s" s="383">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B16" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C16" t="s" s="387">
+        <v>179</v>
+      </c>
+      <c r="D16" t="s" s="384">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s" s="385">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s" s="386">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s" s="388">
+        <v>210</v>
+      </c>
+      <c r="H16" t="s" s="389">
+        <v>21</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="314">
-        <v>127</v>
+      <c r="A17" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B17" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C17" t="s" s="393">
+        <v>180</v>
+      </c>
+      <c r="D17" t="s" s="390">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s" s="391">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s" s="392">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s" s="394">
+        <v>210</v>
+      </c>
+      <c r="H17" t="s" s="395">
+        <v>21</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s" s="322">
-        <v>128</v>
-      </c>
-      <c r="B18" t="s" s="317">
-        <v>129</v>
-      </c>
-      <c r="D18" t="s" s="322">
-        <v>94</v>
-      </c>
-      <c r="E18" t="s" s="317">
-        <v>99</v>
-      </c>
-      <c r="G18" t="s" s="322">
-        <v>96</v>
-      </c>
-      <c r="H18" t="s" s="318">
-        <v>97</v>
+      <c r="A18" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B18" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C18" t="s" s="399">
+        <v>181</v>
+      </c>
+      <c r="D18" t="s" s="396">
+        <v>111</v>
+      </c>
+      <c r="E18" t="s" s="397">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s" s="398">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s" s="400">
+        <v>210</v>
+      </c>
+      <c r="H18" t="s" s="401">
+        <v>211</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="322">
-        <v>130</v>
-      </c>
-      <c r="B19" t="s" s="317">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s" s="322">
-        <v>100</v>
-      </c>
-      <c r="E19" t="s" s="318">
-        <v>131</v>
-      </c>
-      <c r="G19" t="s" s="322">
-        <v>102</v>
-      </c>
-      <c r="H19" t="s" s="318">
-        <v>132</v>
+      <c r="A19" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B19" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C19" t="s" s="405">
+        <v>183</v>
+      </c>
+      <c r="D19" t="s" s="402">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s" s="403">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s" s="404">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s" s="406">
+        <v>210</v>
+      </c>
+      <c r="H19" t="s" s="407">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B20" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C20" t="s" s="411">
+        <v>184</v>
+      </c>
+      <c r="D20" t="s" s="408">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s" s="409">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s" s="410">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s" s="412">
+        <v>210</v>
+      </c>
+      <c r="H20" t="s" s="413">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="421">
+        <v>167</v>
+      </c>
+      <c r="B21" t="s" s="423">
+        <v>168</v>
+      </c>
+      <c r="C21" t="s" s="417">
+        <v>185</v>
+      </c>
+      <c r="D21" t="s" s="414">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s" s="415">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s" s="416">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s" s="418">
+        <v>210</v>
+      </c>
+      <c r="H21" t="s" s="419">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A17:H17"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:A21"/>
+    <mergeCell ref="B6:B21"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Consolidate Allure reporting into unified AllureReportingManager
- Merged DailyAllureManager, AllureEnvironmentInfo, and AllureScreenshotListener
- Created unified AllureReportingManager.java (577 lines)
- Deleted 3 separate files (708 lines total)
- Net reduction: -131 lines (-18.5%)
- Updated all references in Java files and TestNG XML suites
- All functionality preserved: daily reset, environment info, screenshots
- Improved maintainability with single source of truth

Files changed:
  Created: AllureReportingManager.java
  Deleted: DailyAllureManager.java, AllureEnvironmentInfo.java, AllureScreenshotListener.java
  Updated: SuiteHooks.java, ScreenshotHandler.java, Runner02_AddMoreJobsFunctionality.java
  Updated: JAM_SanityTestSuite.xml, JAM_RegressionTestSuite.xml, JAM_SmokeTestSuite.xml
</commit_message>
<xml_diff>
--- a/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
+++ b/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="72">
   <si>
     <t>User Name</t>
   </si>
@@ -157,6 +157,96 @@
   </si>
   <si>
     <t>Find client with access to Profile Manager Application</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>18:22:37</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>3m 39s</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Time: 18:22:37 | Total: 2 | Pass: 0 | Fail: 2</t>
+  </si>
+  <si>
+    <t>Exception: RuntimeException
+Message: Expected condition failed: waiting for element to be clickable: By.xpath: //input[@type='email'] (tried for 90 second(s) with 500 milliseconds interval)
+Build info: version: '4.25.0', revision: '8a8aea2337'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.16'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 133.0.6943.127, chrome: {chromedriverVersion: 133.0.6943.141 (2a5d6da0d61..., userDataDir: C:\Users\navee\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:56769}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:56769/devtoo..., se:cdpVersion: 133.0.6943.127, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 1cbcd4c7e541fcf4553d1d0f45033cd0
+Key Stack Trace:
+  at com.kfonetalentsuite.utils.JobMapping.PageObjectHelper.handleError(PageObjectHelper.java:20)
+  at com.kfonetalentsuite.pageobjects.JobMapping.PO01_KFoneLogin.provide_sso_login_username_and_click_sign_in_button_in_kfone_login_page(PO01_KFoneLogin.java:113)</t>
+  </si>
+  <si>
+    <t>Exception: RuntimeException
+Message: Expected condition failed: waiting for visibility of element located by By.xpath: //table[@id='iam-clients-list-table-content'] (tried for 90 second(s) with 500 milliseconds interval)
+Build info: version: '4.25.0', revision: '8a8aea2337'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.16'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 133.0.6943.127, chrome: {chromedriverVersion: 133.0.6943.141 (2a5d6da0d61..., userDataDir: C:\Users\navee\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:56769}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:56769/devtoo..., se:cdpVersion: 133.0.6943.127, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 1cbcd4c7e541fcf4553d1d0f45033cd0
+Key Stack Trace:
+  at com.kfonetalentsuite.utils.JobMapping.PageObjectHelper.handleError(PageObjectHelper.java:20)
+  at com.kfonetalentsuite.pageobjects.JobMapping.PO01_KFoneLogin.user_is_in_kfone_clients_page(PO01_KFoneLogin.java:228)</t>
+  </si>
+  <si>
+    <t>Test Results Summary - Last Updated: 2025-12-31 18:22:37</t>
+  </si>
+  <si>
+    <t>Daily Status [2025-12-31]: FAILED (1 runs)</t>
+  </si>
+  <si>
+    <t>Passed: 0</t>
+  </si>
+  <si>
+    <t>Failed: 2</t>
+  </si>
+  <si>
+    <t>Duration: 3m 39s</t>
+  </si>
+  <si>
+    <t>19:22:39</t>
+  </si>
+  <si>
+    <t>35s</t>
+  </si>
+  <si>
+    <t>Time: 19:22:39 | Total: 2 | Pass: 2 | Fail: 0</t>
+  </si>
+  <si>
+    <t>Test Results Summary - Last Updated: 2025-12-31 19:22:39</t>
+  </si>
+  <si>
+    <t>Daily Status [2025-12-31]: ALL_PASSED (1 runs)</t>
+  </si>
+  <si>
+    <t>Duration: 35s</t>
+  </si>
+  <si>
+    <t>19:39:30</t>
+  </si>
+  <si>
+    <t>44s</t>
+  </si>
+  <si>
+    <t>Time: 19:39:30 | Total: 2 | Pass: 2 | Fail: 0</t>
+  </si>
+  <si>
+    <t>Test Results Summary - Last Updated: 2025-12-31 19:39:30</t>
+  </si>
+  <si>
+    <t>Duration: 44s</t>
   </si>
 </sst>
 </file>
@@ -164,7 +254,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="17">
+  <fonts count="83">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -244,6 +334,324 @@
     <font>
       <name val="Arial"/>
       <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
     </font>
   </fonts>
   <fills count="10">
@@ -332,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
@@ -393,6 +801,240 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="9" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -406,21 +1048,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="42.3125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="23.4375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.24609375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="16.99609375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="23.4375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="23.4375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.0078125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="18.91015625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="14.96484375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="15.08984375" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.5625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.3125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.4375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0078125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.24609375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.99609375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.4375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.4375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.91015625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.96484375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="15.08984375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.5625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -471,49 +1113,49 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="2">
+      <c r="A2" t="s" s="73">
         <v>15</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" t="s" s="73">
         <v>16</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" t="s" s="73">
         <v>17</v>
       </c>
-      <c r="D2" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s" s="2">
+      <c r="D2" t="s" s="73">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s" s="73">
         <v>19</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="F2" t="s" s="73">
         <v>20</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="G2" t="s" s="73">
         <v>21</v>
       </c>
-      <c r="H2" t="s" s="2">
+      <c r="H2" t="s" s="73">
         <v>22</v>
       </c>
-      <c r="I2" t="n" s="2">
+      <c r="I2" t="n" s="73">
         <v>2.0</v>
       </c>
-      <c r="J2" t="n" s="2">
+      <c r="J2" t="n" s="73">
         <v>2.0</v>
       </c>
-      <c r="K2" t="n" s="2">
+      <c r="K2" t="n" s="73">
         <v>0.0</v>
       </c>
-      <c r="L2" t="n" s="2">
+      <c r="L2" t="n" s="73">
         <v>0.0</v>
       </c>
-      <c r="M2" t="s" s="2">
+      <c r="M2" t="s" s="73">
         <v>23</v>
       </c>
-      <c r="N2" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="O2" t="s" s="3">
+      <c r="N2" t="s" s="73">
+        <v>68</v>
+      </c>
+      <c r="O2" t="s" s="74">
         <v>25</v>
       </c>
     </row>
@@ -530,24 +1172,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.0625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="69.60546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="43.28125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.71875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.75" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="34.109375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="22.34375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.0625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="69.60546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="43.28125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.71875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.75"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="34.109375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.34375"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="4">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>28</v>
@@ -562,7 +1204,7 @@
         <v>31</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>32</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -592,59 +1234,59 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="17">
+      <c r="A6" t="s" s="87">
         <v>41</v>
       </c>
-      <c r="B6" t="s" s="19">
+      <c r="B6" t="s" s="89">
         <v>42</v>
       </c>
-      <c r="C6" t="s" s="8">
+      <c r="C6" t="s" s="91">
         <v>43</v>
       </c>
-      <c r="D6" t="s" s="5">
+      <c r="D6" t="s" s="92">
         <v>25</v>
       </c>
-      <c r="E6" t="s" s="6">
+      <c r="E6" t="s" s="93">
         <v>44</v>
       </c>
-      <c r="F6" t="s" s="7">
+      <c r="F6" t="s" s="94">
         <v>44</v>
       </c>
-      <c r="G6" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="H6" t="s" s="10">
+      <c r="G6" t="s" s="91">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s" s="91">
         <v>46</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="17">
+      <c r="A7" t="s" s="87">
         <v>41</v>
       </c>
-      <c r="B7" t="s" s="19">
+      <c r="B7" t="s" s="89">
         <v>42</v>
       </c>
-      <c r="C7" t="s" s="14">
+      <c r="C7" t="s" s="95">
         <v>47</v>
       </c>
-      <c r="D7" t="s" s="11">
+      <c r="D7" t="s" s="96">
         <v>25</v>
       </c>
-      <c r="E7" t="s" s="12">
+      <c r="E7" t="s" s="97">
         <v>44</v>
       </c>
-      <c r="F7" t="s" s="13">
+      <c r="F7" t="s" s="98">
         <v>44</v>
       </c>
-      <c r="G7" t="s" s="15">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s" s="16">
+      <c r="G7" t="s" s="95">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s" s="95">
         <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>

</xml_diff>

<commit_message>
Remove search retry/attempt logic from PO06 - simplified search_for_published_job_name1 and name2, removed 3 search attempts + 5 verification retries per search
</commit_message>
<xml_diff>
--- a/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
+++ b/e2e-automation/ExcelReports/JobMappingAutomationTestResults.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="226">
   <si>
     <t>User Name</t>
   </si>
@@ -721,13 +721,28 @@
   <si>
     <t>Duration: 9m 11s</t>
   </si>
+  <si>
+    <t>12:37:00</t>
+  </si>
+  <si>
+    <t>8m 16s</t>
+  </si>
+  <si>
+    <t>Time: 12:37:00 | Total: 20 | Pass: 20 | Fail: 0</t>
+  </si>
+  <si>
+    <t>Test Results Summary - Last Updated: 2026-01-02 12:37:00</t>
+  </si>
+  <si>
+    <t>Duration: 8m 16s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1908">
+  <fonts count="2234">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -7535,6 +7550,1658 @@
     <font>
       <name val="Arial"/>
       <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <color indexed="58"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -10385,7 +12052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1956">
+  <cellXfs count="2286">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
@@ -16250,6 +17917,996 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1907" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1908" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1909" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1910" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1911" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1912" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1913" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1914" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1915" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1916" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1917" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1918" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1919" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1920" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1921" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1922" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1923" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1924" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1925" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1926" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1927" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1928" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1929" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1930" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1931" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1932" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1933" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1934" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1935" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1936" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1937" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1938" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1939" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1940" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1941" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1942" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1943" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1944" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1945" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1946" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1947" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1948" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1949" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1950" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1951" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1952" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1953" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1954" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1955" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1956" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1957" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1958" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1959" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1960" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1961" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1962" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1963" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1964" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1965" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1966" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1967" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1968" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1969" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1970" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1971" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1972" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1973" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1974" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1975" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1976" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1977" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1978" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1979" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1980" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1981" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1982" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1983" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1984" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1985" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1986" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1987" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1988" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1989" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1990" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1991" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1992" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1993" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1994" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1995" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1996" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1997" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1998" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1999" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2000" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2001" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2002" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2003" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2004" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2005" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2006" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2007" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2008" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2009" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2010" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2011" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2012" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2013" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2014" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2015" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2016" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2017" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2018" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2019" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2020" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2021" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2022" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2023" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2024" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2025" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2026" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2027" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2028" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2029" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2030" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2031" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2032" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2033" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2034" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2035" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2036" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2037" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2038" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2039" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2040" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2041" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2042" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2043" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2044" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2045" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2046" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2047" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2048" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2049" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2050" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2051" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2052" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2053" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2054" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2055" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2056" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2057" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2058" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2059" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2060" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2061" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2062" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2063" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2064" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2065" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2066" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2067" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2068" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2069" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2070" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2071" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2072" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2073" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2074" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2075" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2076" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2077" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2078" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2079" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2080" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2081" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2082" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2083" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2084" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2085" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2086" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2087" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2088" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2089" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2090" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2091" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2092" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2093" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2094" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2095" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2096" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2097" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2098" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2099" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2100" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2101" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2102" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2103" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2104" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2105" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2106" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2107" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2108" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2109" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2110" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2111" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2112" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2113" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2114" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2115" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2116" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2117" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2118" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2119" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2120" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2121" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2122" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2123" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2124" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2125" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2126" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2127" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2128" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2129" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2130" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2131" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2132" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2133" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2134" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2135" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2136" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2137" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2138" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2139" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2140" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2141" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2142" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2143" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2144" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2145" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2146" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2147" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2148" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2149" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2150" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2151" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2152" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2153" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2154" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2155" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2156" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2157" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2158" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2159" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2160" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2161" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2162" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2163" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2164" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2165" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2166" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2167" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2168" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2169" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2170" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2171" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2172" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2173" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2174" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2175" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2176" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2177" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2178" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2179" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2180" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2181" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2182" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2183" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2184" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2185" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2186" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2187" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2188" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2189" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2190" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2191" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2192" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2193" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2194" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2195" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2196" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2197" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2198" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2199" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2200" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2201" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2202" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2203" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2204" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2205" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2206" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2207" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2208" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2209" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2210" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2211" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2212" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2213" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2214" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2215" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2216" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2217" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2218" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2219" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2220" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2221" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2222" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2223" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2224" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2225" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2226" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2227" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2228" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2229" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2230" fillId="5" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2231" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2232" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2233" fillId="5" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -16658,49 +19315,49 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="1626">
+      <c r="A9" t="s" s="1956">
         <v>15</v>
       </c>
-      <c r="B9" t="s" s="1626">
+      <c r="B9" t="s" s="1956">
         <v>16</v>
       </c>
-      <c r="C9" t="s" s="1626">
+      <c r="C9" t="s" s="1956">
         <v>98</v>
       </c>
-      <c r="D9" t="s" s="1626">
-        <v>213</v>
-      </c>
-      <c r="E9" t="s" s="1626">
+      <c r="D9" t="s" s="1956">
+        <v>221</v>
+      </c>
+      <c r="E9" t="s" s="1956">
         <v>19</v>
       </c>
-      <c r="F9" t="s" s="1626">
+      <c r="F9" t="s" s="1956">
         <v>20</v>
       </c>
-      <c r="G9" t="s" s="1626">
+      <c r="G9" t="s" s="1956">
         <v>21</v>
       </c>
-      <c r="H9" t="s" s="1626">
+      <c r="H9" t="s" s="1956">
         <v>173</v>
       </c>
-      <c r="I9" t="n" s="1626">
+      <c r="I9" t="n" s="1956">
         <v>20.0</v>
       </c>
-      <c r="J9" t="n" s="1626">
+      <c r="J9" t="n" s="1956">
         <v>20.0</v>
       </c>
-      <c r="K9" t="n" s="1626">
+      <c r="K9" t="n" s="1956">
         <v>0.0</v>
       </c>
-      <c r="L9" t="n" s="1626">
+      <c r="L9" t="n" s="1956">
         <v>0.0</v>
       </c>
-      <c r="M9" t="s" s="1626">
+      <c r="M9" t="s" s="1956">
         <v>23</v>
       </c>
-      <c r="N9" t="s" s="1626">
-        <v>214</v>
-      </c>
-      <c r="O9" t="s" s="1627">
+      <c r="N9" t="s" s="1956">
+        <v>222</v>
+      </c>
+      <c r="O9" t="s" s="1957">
         <v>25</v>
       </c>
     </row>
@@ -16729,7 +19386,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="413">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3">
@@ -16749,7 +19406,7 @@
         <v>31</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5">
@@ -16779,1333 +19436,1333 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="1748">
+      <c r="A6" t="s" s="2078">
         <v>41</v>
       </c>
-      <c r="B6" t="s" s="1750">
+      <c r="B6" t="s" s="2080">
         <v>42</v>
       </c>
-      <c r="C6" t="s" s="1752">
+      <c r="C6" t="s" s="2082">
         <v>43</v>
       </c>
-      <c r="D6" t="s" s="1753">
+      <c r="D6" t="s" s="2083">
         <v>25</v>
       </c>
-      <c r="E6" t="s" s="1754">
+      <c r="E6" t="s" s="2084">
         <v>44</v>
       </c>
-      <c r="F6" t="s" s="1755">
+      <c r="F6" t="s" s="2085">
         <v>44</v>
       </c>
-      <c r="G6" t="s" s="1752">
+      <c r="G6" t="s" s="2082">
         <v>104</v>
       </c>
-      <c r="H6" t="s" s="1752">
+      <c r="H6" t="s" s="2082">
         <v>46</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="1748">
+      <c r="A7" t="s" s="2078">
         <v>41</v>
       </c>
-      <c r="B7" t="s" s="1750">
+      <c r="B7" t="s" s="2080">
         <v>42</v>
       </c>
-      <c r="C7" t="s" s="1756">
+      <c r="C7" t="s" s="2086">
         <v>47</v>
       </c>
-      <c r="D7" t="s" s="1757">
+      <c r="D7" t="s" s="2087">
         <v>25</v>
       </c>
-      <c r="E7" t="s" s="1758">
+      <c r="E7" t="s" s="2088">
         <v>44</v>
       </c>
-      <c r="F7" t="s" s="1759">
+      <c r="F7" t="s" s="2089">
         <v>44</v>
       </c>
-      <c r="G7" t="s" s="1756">
+      <c r="G7" t="s" s="2086">
         <v>104</v>
       </c>
-      <c r="H7" t="s" s="1756">
+      <c r="H7" t="s" s="2086">
         <v>46</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="1748">
+      <c r="A8" t="s" s="2078">
         <v>110</v>
       </c>
-      <c r="B8" t="s" s="1750">
+      <c r="B8" t="s" s="2080">
         <v>111</v>
       </c>
-      <c r="C8" t="s" s="1760">
+      <c r="C8" t="s" s="2090">
         <v>43</v>
       </c>
-      <c r="D8" t="s" s="1761">
+      <c r="D8" t="s" s="2091">
         <v>25</v>
       </c>
-      <c r="E8" t="s" s="1762">
+      <c r="E8" t="s" s="2092">
         <v>44</v>
       </c>
-      <c r="F8" t="s" s="1763">
+      <c r="F8" t="s" s="2093">
         <v>44</v>
       </c>
-      <c r="G8" t="s" s="1760">
+      <c r="G8" t="s" s="2090">
         <v>130</v>
       </c>
-      <c r="H8" t="s" s="1760">
+      <c r="H8" t="s" s="2090">
         <v>46</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="1748">
+      <c r="A9" t="s" s="2078">
         <v>110</v>
       </c>
-      <c r="B9" t="s" s="1750">
+      <c r="B9" t="s" s="2080">
         <v>111</v>
       </c>
-      <c r="C9" t="s" s="1764">
+      <c r="C9" t="s" s="2094">
         <v>47</v>
       </c>
-      <c r="D9" t="s" s="1765">
+      <c r="D9" t="s" s="2095">
         <v>25</v>
       </c>
-      <c r="E9" t="s" s="1766">
+      <c r="E9" t="s" s="2096">
         <v>44</v>
       </c>
-      <c r="F9" t="s" s="1767">
+      <c r="F9" t="s" s="2097">
         <v>44</v>
       </c>
-      <c r="G9" t="s" s="1764">
+      <c r="G9" t="s" s="2094">
         <v>130</v>
       </c>
-      <c r="H9" t="s" s="1764">
+      <c r="H9" t="s" s="2094">
         <v>46</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="1748">
+      <c r="A10" t="s" s="2078">
         <v>110</v>
       </c>
-      <c r="B10" t="s" s="1750">
+      <c r="B10" t="s" s="2080">
         <v>111</v>
       </c>
-      <c r="C10" t="s" s="1768">
+      <c r="C10" t="s" s="2098">
         <v>67</v>
       </c>
-      <c r="D10" t="s" s="1769">
+      <c r="D10" t="s" s="2099">
         <v>25</v>
       </c>
-      <c r="E10" t="s" s="1770">
+      <c r="E10" t="s" s="2100">
         <v>44</v>
       </c>
-      <c r="F10" t="s" s="1771">
+      <c r="F10" t="s" s="2101">
         <v>44</v>
       </c>
-      <c r="G10" t="s" s="1768">
+      <c r="G10" t="s" s="2098">
         <v>130</v>
       </c>
-      <c r="H10" t="s" s="1768">
+      <c r="H10" t="s" s="2098">
         <v>46</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="1748">
+      <c r="A11" t="s" s="2078">
         <v>110</v>
       </c>
-      <c r="B11" t="s" s="1750">
+      <c r="B11" t="s" s="2080">
         <v>111</v>
       </c>
-      <c r="C11" t="s" s="1772">
+      <c r="C11" t="s" s="2102">
         <v>113</v>
       </c>
-      <c r="D11" t="s" s="1773">
+      <c r="D11" t="s" s="2103">
         <v>25</v>
       </c>
-      <c r="E11" t="s" s="1774">
+      <c r="E11" t="s" s="2104">
         <v>44</v>
       </c>
-      <c r="F11" t="s" s="1775">
+      <c r="F11" t="s" s="2105">
         <v>44</v>
       </c>
-      <c r="G11" t="s" s="1772">
+      <c r="G11" t="s" s="2102">
         <v>130</v>
       </c>
-      <c r="H11" t="s" s="1772">
+      <c r="H11" t="s" s="2102">
         <v>46</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s" s="1748">
+      <c r="A12" t="s" s="2078">
         <v>110</v>
       </c>
-      <c r="B12" t="s" s="1750">
+      <c r="B12" t="s" s="2080">
         <v>111</v>
       </c>
-      <c r="C12" t="s" s="1776">
+      <c r="C12" t="s" s="2106">
         <v>114</v>
       </c>
-      <c r="D12" t="s" s="1777">
+      <c r="D12" t="s" s="2107">
         <v>25</v>
       </c>
-      <c r="E12" t="s" s="1778">
+      <c r="E12" t="s" s="2108">
         <v>44</v>
       </c>
-      <c r="F12" t="s" s="1779">
+      <c r="F12" t="s" s="2109">
         <v>44</v>
       </c>
-      <c r="G12" t="s" s="1776">
+      <c r="G12" t="s" s="2106">
         <v>130</v>
       </c>
-      <c r="H12" t="s" s="1776">
+      <c r="H12" t="s" s="2106">
         <v>46</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="1748">
+      <c r="A13" t="s" s="2078">
         <v>110</v>
       </c>
-      <c r="B13" t="s" s="1750">
+      <c r="B13" t="s" s="2080">
         <v>111</v>
       </c>
-      <c r="C13" t="s" s="1780">
+      <c r="C13" t="s" s="2110">
         <v>115</v>
       </c>
-      <c r="D13" t="s" s="1781">
+      <c r="D13" t="s" s="2111">
         <v>25</v>
       </c>
-      <c r="E13" t="s" s="1782">
+      <c r="E13" t="s" s="2112">
         <v>44</v>
       </c>
-      <c r="F13" t="s" s="1783">
+      <c r="F13" t="s" s="2113">
         <v>44</v>
       </c>
-      <c r="G13" t="s" s="1780">
+      <c r="G13" t="s" s="2110">
         <v>130</v>
       </c>
-      <c r="H13" t="s" s="1780">
+      <c r="H13" t="s" s="2110">
         <v>46</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="1748">
+      <c r="A14" t="s" s="2078">
         <v>138</v>
       </c>
-      <c r="B14" t="s" s="1750">
+      <c r="B14" t="s" s="2080">
         <v>139</v>
       </c>
-      <c r="C14" t="s" s="1784">
+      <c r="C14" t="s" s="2114">
         <v>43</v>
       </c>
-      <c r="D14" t="s" s="1785">
+      <c r="D14" t="s" s="2115">
         <v>25</v>
       </c>
-      <c r="E14" t="s" s="1786">
+      <c r="E14" t="s" s="2116">
         <v>44</v>
       </c>
-      <c r="F14" t="s" s="1787">
+      <c r="F14" t="s" s="2117">
         <v>44</v>
       </c>
-      <c r="G14" t="s" s="1784">
+      <c r="G14" t="s" s="2114">
         <v>140</v>
       </c>
-      <c r="H14" t="s" s="1784">
+      <c r="H14" t="s" s="2114">
         <v>46</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="1748">
+      <c r="A15" t="s" s="2078">
         <v>138</v>
       </c>
-      <c r="B15" t="s" s="1750">
+      <c r="B15" t="s" s="2080">
         <v>139</v>
       </c>
-      <c r="C15" t="s" s="1788">
+      <c r="C15" t="s" s="2118">
         <v>47</v>
       </c>
-      <c r="D15" t="s" s="1789">
+      <c r="D15" t="s" s="2119">
         <v>25</v>
       </c>
-      <c r="E15" t="s" s="1790">
+      <c r="E15" t="s" s="2120">
         <v>44</v>
       </c>
-      <c r="F15" t="s" s="1791">
+      <c r="F15" t="s" s="2121">
         <v>44</v>
       </c>
-      <c r="G15" t="s" s="1788">
+      <c r="G15" t="s" s="2118">
         <v>140</v>
       </c>
-      <c r="H15" t="s" s="1788">
+      <c r="H15" t="s" s="2118">
         <v>46</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s" s="1748">
+      <c r="A16" t="s" s="2078">
         <v>138</v>
       </c>
-      <c r="B16" t="s" s="1750">
+      <c r="B16" t="s" s="2080">
         <v>139</v>
       </c>
-      <c r="C16" t="s" s="1792">
+      <c r="C16" t="s" s="2122">
         <v>67</v>
       </c>
-      <c r="D16" t="s" s="1793">
+      <c r="D16" t="s" s="2123">
         <v>25</v>
       </c>
-      <c r="E16" t="s" s="1794">
+      <c r="E16" t="s" s="2124">
         <v>44</v>
       </c>
-      <c r="F16" t="s" s="1795">
+      <c r="F16" t="s" s="2125">
         <v>44</v>
       </c>
-      <c r="G16" t="s" s="1792">
+      <c r="G16" t="s" s="2122">
         <v>140</v>
       </c>
-      <c r="H16" t="s" s="1792">
+      <c r="H16" t="s" s="2122">
         <v>46</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="1748">
+      <c r="A17" t="s" s="2078">
         <v>138</v>
       </c>
-      <c r="B17" t="s" s="1750">
+      <c r="B17" t="s" s="2080">
         <v>139</v>
       </c>
-      <c r="C17" t="s" s="1796">
+      <c r="C17" t="s" s="2126">
         <v>141</v>
       </c>
-      <c r="D17" t="s" s="1797">
+      <c r="D17" t="s" s="2127">
         <v>25</v>
       </c>
-      <c r="E17" t="s" s="1798">
+      <c r="E17" t="s" s="2128">
         <v>44</v>
       </c>
-      <c r="F17" t="s" s="1799">
+      <c r="F17" t="s" s="2129">
         <v>44</v>
       </c>
-      <c r="G17" t="s" s="1796">
+      <c r="G17" t="s" s="2126">
         <v>140</v>
       </c>
-      <c r="H17" t="s" s="1796">
+      <c r="H17" t="s" s="2126">
         <v>46</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s" s="1748">
+      <c r="A18" t="s" s="2078">
         <v>138</v>
       </c>
-      <c r="B18" t="s" s="1750">
+      <c r="B18" t="s" s="2080">
         <v>139</v>
       </c>
-      <c r="C18" t="s" s="1800">
+      <c r="C18" t="s" s="2130">
         <v>142</v>
       </c>
-      <c r="D18" t="s" s="1801">
+      <c r="D18" t="s" s="2131">
         <v>25</v>
       </c>
-      <c r="E18" t="s" s="1802">
+      <c r="E18" t="s" s="2132">
         <v>44</v>
       </c>
-      <c r="F18" t="s" s="1803">
+      <c r="F18" t="s" s="2133">
         <v>44</v>
       </c>
-      <c r="G18" t="s" s="1800">
+      <c r="G18" t="s" s="2130">
         <v>140</v>
       </c>
-      <c r="H18" t="s" s="1800">
+      <c r="H18" t="s" s="2130">
         <v>46</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="1748">
+      <c r="A19" t="s" s="2078">
         <v>138</v>
       </c>
-      <c r="B19" t="s" s="1750">
+      <c r="B19" t="s" s="2080">
         <v>139</v>
       </c>
-      <c r="C19" t="s" s="1804">
+      <c r="C19" t="s" s="2134">
         <v>143</v>
       </c>
-      <c r="D19" t="s" s="1805">
+      <c r="D19" t="s" s="2135">
         <v>25</v>
       </c>
-      <c r="E19" t="s" s="1806">
+      <c r="E19" t="s" s="2136">
         <v>44</v>
       </c>
-      <c r="F19" t="s" s="1807">
+      <c r="F19" t="s" s="2137">
         <v>44</v>
       </c>
-      <c r="G19" t="s" s="1804">
+      <c r="G19" t="s" s="2134">
         <v>140</v>
       </c>
-      <c r="H19" t="s" s="1804">
+      <c r="H19" t="s" s="2134">
         <v>46</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s" s="1748">
+      <c r="A20" t="s" s="2078">
         <v>138</v>
       </c>
-      <c r="B20" t="s" s="1750">
+      <c r="B20" t="s" s="2080">
         <v>139</v>
       </c>
-      <c r="C20" t="s" s="1808">
+      <c r="C20" t="s" s="2138">
         <v>144</v>
       </c>
-      <c r="D20" t="s" s="1809">
+      <c r="D20" t="s" s="2139">
         <v>25</v>
       </c>
-      <c r="E20" t="s" s="1810">
+      <c r="E20" t="s" s="2140">
         <v>44</v>
       </c>
-      <c r="F20" t="s" s="1811">
+      <c r="F20" t="s" s="2141">
         <v>44</v>
       </c>
-      <c r="G20" t="s" s="1808">
+      <c r="G20" t="s" s="2138">
         <v>140</v>
       </c>
-      <c r="H20" t="s" s="1808">
+      <c r="H20" t="s" s="2138">
         <v>46</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s" s="1748">
+      <c r="A21" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B21" t="s" s="1750">
+      <c r="B21" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C21" t="s" s="1812">
+      <c r="C21" t="s" s="2142">
         <v>43</v>
       </c>
-      <c r="D21" t="s" s="1813">
+      <c r="D21" t="s" s="2143">
         <v>25</v>
       </c>
-      <c r="E21" t="s" s="1814">
+      <c r="E21" t="s" s="2144">
         <v>44</v>
       </c>
-      <c r="F21" t="s" s="1815">
+      <c r="F21" t="s" s="2145">
         <v>44</v>
       </c>
-      <c r="G21" t="s" s="1812">
+      <c r="G21" t="s" s="2142">
         <v>154</v>
       </c>
-      <c r="H21" t="s" s="1812">
+      <c r="H21" t="s" s="2142">
         <v>46</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s" s="1748">
+      <c r="A22" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B22" t="s" s="1750">
+      <c r="B22" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C22" t="s" s="1816">
+      <c r="C22" t="s" s="2146">
         <v>47</v>
       </c>
-      <c r="D22" t="s" s="1817">
+      <c r="D22" t="s" s="2147">
         <v>25</v>
       </c>
-      <c r="E22" t="s" s="1818">
+      <c r="E22" t="s" s="2148">
         <v>44</v>
       </c>
-      <c r="F22" t="s" s="1819">
+      <c r="F22" t="s" s="2149">
         <v>44</v>
       </c>
-      <c r="G22" t="s" s="1816">
+      <c r="G22" t="s" s="2146">
         <v>154</v>
       </c>
-      <c r="H22" t="s" s="1816">
+      <c r="H22" t="s" s="2146">
         <v>46</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s" s="1748">
+      <c r="A23" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B23" t="s" s="1750">
+      <c r="B23" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C23" t="s" s="1820">
+      <c r="C23" t="s" s="2150">
         <v>67</v>
       </c>
-      <c r="D23" t="s" s="1821">
+      <c r="D23" t="s" s="2151">
         <v>25</v>
       </c>
-      <c r="E23" t="s" s="1822">
+      <c r="E23" t="s" s="2152">
         <v>44</v>
       </c>
-      <c r="F23" t="s" s="1823">
+      <c r="F23" t="s" s="2153">
         <v>44</v>
       </c>
-      <c r="G23" t="s" s="1820">
+      <c r="G23" t="s" s="2150">
         <v>154</v>
       </c>
-      <c r="H23" t="s" s="1820">
+      <c r="H23" t="s" s="2150">
         <v>46</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s" s="1748">
+      <c r="A24" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B24" t="s" s="1750">
+      <c r="B24" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C24" t="s" s="1824">
+      <c r="C24" t="s" s="2154">
         <v>155</v>
       </c>
-      <c r="D24" t="s" s="1825">
+      <c r="D24" t="s" s="2155">
         <v>25</v>
       </c>
-      <c r="E24" t="s" s="1826">
+      <c r="E24" t="s" s="2156">
         <v>44</v>
       </c>
-      <c r="F24" t="s" s="1827">
+      <c r="F24" t="s" s="2157">
         <v>44</v>
       </c>
-      <c r="G24" t="s" s="1824">
+      <c r="G24" t="s" s="2154">
         <v>154</v>
       </c>
-      <c r="H24" t="s" s="1824">
+      <c r="H24" t="s" s="2154">
         <v>46</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="1748">
+      <c r="A25" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B25" t="s" s="1750">
+      <c r="B25" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C25" t="s" s="1828">
+      <c r="C25" t="s" s="2158">
         <v>156</v>
       </c>
-      <c r="D25" t="s" s="1829">
+      <c r="D25" t="s" s="2159">
         <v>25</v>
       </c>
-      <c r="E25" t="s" s="1830">
+      <c r="E25" t="s" s="2160">
         <v>44</v>
       </c>
-      <c r="F25" t="s" s="1831">
+      <c r="F25" t="s" s="2161">
         <v>44</v>
       </c>
-      <c r="G25" t="s" s="1828">
+      <c r="G25" t="s" s="2158">
         <v>154</v>
       </c>
-      <c r="H25" t="s" s="1828">
+      <c r="H25" t="s" s="2158">
         <v>46</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s" s="1748">
+      <c r="A26" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B26" t="s" s="1750">
+      <c r="B26" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C26" t="s" s="1832">
+      <c r="C26" t="s" s="2162">
         <v>157</v>
       </c>
-      <c r="D26" t="s" s="1833">
+      <c r="D26" t="s" s="2163">
         <v>25</v>
       </c>
-      <c r="E26" t="s" s="1834">
+      <c r="E26" t="s" s="2164">
         <v>44</v>
       </c>
-      <c r="F26" t="s" s="1835">
+      <c r="F26" t="s" s="2165">
         <v>44</v>
       </c>
-      <c r="G26" t="s" s="1832">
+      <c r="G26" t="s" s="2162">
         <v>154</v>
       </c>
-      <c r="H26" t="s" s="1832">
+      <c r="H26" t="s" s="2162">
         <v>46</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="1748">
+      <c r="A27" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B27" t="s" s="1750">
+      <c r="B27" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C27" t="s" s="1836">
+      <c r="C27" t="s" s="2166">
         <v>158</v>
       </c>
-      <c r="D27" t="s" s="1837">
+      <c r="D27" t="s" s="2167">
         <v>25</v>
       </c>
-      <c r="E27" t="s" s="1838">
+      <c r="E27" t="s" s="2168">
         <v>44</v>
       </c>
-      <c r="F27" t="s" s="1839">
+      <c r="F27" t="s" s="2169">
         <v>44</v>
       </c>
-      <c r="G27" t="s" s="1836">
+      <c r="G27" t="s" s="2166">
         <v>154</v>
       </c>
-      <c r="H27" t="s" s="1836">
+      <c r="H27" t="s" s="2166">
         <v>46</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s" s="1748">
+      <c r="A28" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B28" t="s" s="1750">
+      <c r="B28" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C28" t="s" s="1840">
+      <c r="C28" t="s" s="2170">
         <v>159</v>
       </c>
-      <c r="D28" t="s" s="1841">
+      <c r="D28" t="s" s="2171">
         <v>25</v>
       </c>
-      <c r="E28" t="s" s="1842">
+      <c r="E28" t="s" s="2172">
         <v>44</v>
       </c>
-      <c r="F28" t="s" s="1843">
+      <c r="F28" t="s" s="2173">
         <v>44</v>
       </c>
-      <c r="G28" t="s" s="1840">
+      <c r="G28" t="s" s="2170">
         <v>154</v>
       </c>
-      <c r="H28" t="s" s="1840">
+      <c r="H28" t="s" s="2170">
         <v>46</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s" s="1748">
+      <c r="A29" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B29" t="s" s="1750">
+      <c r="B29" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C29" t="s" s="1844">
+      <c r="C29" t="s" s="2174">
         <v>160</v>
       </c>
-      <c r="D29" t="s" s="1845">
+      <c r="D29" t="s" s="2175">
         <v>25</v>
       </c>
-      <c r="E29" t="s" s="1846">
+      <c r="E29" t="s" s="2176">
         <v>44</v>
       </c>
-      <c r="F29" t="s" s="1847">
+      <c r="F29" t="s" s="2177">
         <v>44</v>
       </c>
-      <c r="G29" t="s" s="1844">
+      <c r="G29" t="s" s="2174">
         <v>154</v>
       </c>
-      <c r="H29" t="s" s="1844">
+      <c r="H29" t="s" s="2174">
         <v>46</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s" s="1748">
+      <c r="A30" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B30" t="s" s="1750">
+      <c r="B30" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C30" t="s" s="1848">
+      <c r="C30" t="s" s="2178">
         <v>161</v>
       </c>
-      <c r="D30" t="s" s="1849">
+      <c r="D30" t="s" s="2179">
         <v>25</v>
       </c>
-      <c r="E30" t="s" s="1850">
+      <c r="E30" t="s" s="2180">
         <v>44</v>
       </c>
-      <c r="F30" t="s" s="1851">
+      <c r="F30" t="s" s="2181">
         <v>44</v>
       </c>
-      <c r="G30" t="s" s="1848">
+      <c r="G30" t="s" s="2178">
         <v>154</v>
       </c>
-      <c r="H30" t="s" s="1848">
+      <c r="H30" t="s" s="2178">
         <v>46</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s" s="1748">
+      <c r="A31" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B31" t="s" s="1750">
+      <c r="B31" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C31" t="s" s="1852">
+      <c r="C31" t="s" s="2182">
         <v>162</v>
       </c>
-      <c r="D31" t="s" s="1853">
+      <c r="D31" t="s" s="2183">
         <v>25</v>
       </c>
-      <c r="E31" t="s" s="1854">
+      <c r="E31" t="s" s="2184">
         <v>44</v>
       </c>
-      <c r="F31" t="s" s="1855">
+      <c r="F31" t="s" s="2185">
         <v>44</v>
       </c>
-      <c r="G31" t="s" s="1852">
+      <c r="G31" t="s" s="2182">
         <v>154</v>
       </c>
-      <c r="H31" t="s" s="1852">
+      <c r="H31" t="s" s="2182">
         <v>46</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s" s="1748">
+      <c r="A32" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B32" t="s" s="1750">
+      <c r="B32" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C32" t="s" s="1856">
+      <c r="C32" t="s" s="2186">
         <v>163</v>
       </c>
-      <c r="D32" t="s" s="1857">
+      <c r="D32" t="s" s="2187">
         <v>25</v>
       </c>
-      <c r="E32" t="s" s="1858">
+      <c r="E32" t="s" s="2188">
         <v>44</v>
       </c>
-      <c r="F32" t="s" s="1859">
+      <c r="F32" t="s" s="2189">
         <v>44</v>
       </c>
-      <c r="G32" t="s" s="1856">
+      <c r="G32" t="s" s="2186">
         <v>154</v>
       </c>
-      <c r="H32" t="s" s="1856">
+      <c r="H32" t="s" s="2186">
         <v>46</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s" s="1748">
+      <c r="A33" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B33" t="s" s="1750">
+      <c r="B33" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C33" t="s" s="1860">
+      <c r="C33" t="s" s="2190">
         <v>164</v>
       </c>
-      <c r="D33" t="s" s="1861">
+      <c r="D33" t="s" s="2191">
         <v>25</v>
       </c>
-      <c r="E33" t="s" s="1862">
+      <c r="E33" t="s" s="2192">
         <v>44</v>
       </c>
-      <c r="F33" t="s" s="1863">
+      <c r="F33" t="s" s="2193">
         <v>44</v>
       </c>
-      <c r="G33" t="s" s="1860">
+      <c r="G33" t="s" s="2190">
         <v>154</v>
       </c>
-      <c r="H33" t="s" s="1860">
+      <c r="H33" t="s" s="2190">
         <v>46</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s" s="1748">
+      <c r="A34" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B34" t="s" s="1750">
+      <c r="B34" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C34" t="s" s="1864">
+      <c r="C34" t="s" s="2194">
         <v>165</v>
       </c>
-      <c r="D34" t="s" s="1865">
+      <c r="D34" t="s" s="2195">
         <v>25</v>
       </c>
-      <c r="E34" t="s" s="1866">
+      <c r="E34" t="s" s="2196">
         <v>44</v>
       </c>
-      <c r="F34" t="s" s="1867">
+      <c r="F34" t="s" s="2197">
         <v>44</v>
       </c>
-      <c r="G34" t="s" s="1864">
+      <c r="G34" t="s" s="2194">
         <v>154</v>
       </c>
-      <c r="H34" t="s" s="1864">
+      <c r="H34" t="s" s="2194">
         <v>46</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s" s="1748">
+      <c r="A35" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B35" t="s" s="1750">
+      <c r="B35" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C35" t="s" s="1868">
+      <c r="C35" t="s" s="2198">
         <v>166</v>
       </c>
-      <c r="D35" t="s" s="1869">
+      <c r="D35" t="s" s="2199">
         <v>25</v>
       </c>
-      <c r="E35" t="s" s="1870">
+      <c r="E35" t="s" s="2200">
         <v>44</v>
       </c>
-      <c r="F35" t="s" s="1871">
+      <c r="F35" t="s" s="2201">
         <v>44</v>
       </c>
-      <c r="G35" t="s" s="1868">
+      <c r="G35" t="s" s="2198">
         <v>154</v>
       </c>
-      <c r="H35" t="s" s="1868">
+      <c r="H35" t="s" s="2198">
         <v>46</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s" s="1748">
+      <c r="A36" t="s" s="2078">
         <v>152</v>
       </c>
-      <c r="B36" t="s" s="1750">
+      <c r="B36" t="s" s="2080">
         <v>153</v>
       </c>
-      <c r="C36" t="s" s="1872">
+      <c r="C36" t="s" s="2202">
         <v>167</v>
       </c>
-      <c r="D36" t="s" s="1873">
+      <c r="D36" t="s" s="2203">
         <v>25</v>
       </c>
-      <c r="E36" t="s" s="1874">
+      <c r="E36" t="s" s="2204">
         <v>44</v>
       </c>
-      <c r="F36" t="s" s="1875">
+      <c r="F36" t="s" s="2205">
         <v>44</v>
       </c>
-      <c r="G36" t="s" s="1872">
+      <c r="G36" t="s" s="2202">
         <v>154</v>
       </c>
-      <c r="H36" t="s" s="1872">
+      <c r="H36" t="s" s="2202">
         <v>46</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s" s="1748">
+      <c r="A37" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B37" t="s" s="1750">
+      <c r="B37" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C37" t="s" s="1876">
+      <c r="C37" t="s" s="2206">
         <v>43</v>
       </c>
-      <c r="D37" t="s" s="1877">
+      <c r="D37" t="s" s="2207">
         <v>25</v>
       </c>
-      <c r="E37" t="s" s="1878">
+      <c r="E37" t="s" s="2208">
         <v>44</v>
       </c>
-      <c r="F37" t="s" s="1879">
+      <c r="F37" t="s" s="2209">
         <v>44</v>
       </c>
-      <c r="G37" t="s" s="1876">
-        <v>215</v>
-      </c>
-      <c r="H37" t="s" s="1876">
+      <c r="G37" t="s" s="2206">
+        <v>223</v>
+      </c>
+      <c r="H37" t="s" s="2206">
         <v>46</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s" s="1748">
+      <c r="A38" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B38" t="s" s="1750">
+      <c r="B38" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C38" t="s" s="1880">
+      <c r="C38" t="s" s="2210">
         <v>47</v>
       </c>
-      <c r="D38" t="s" s="1881">
+      <c r="D38" t="s" s="2211">
         <v>25</v>
       </c>
-      <c r="E38" t="s" s="1882">
+      <c r="E38" t="s" s="2212">
         <v>44</v>
       </c>
-      <c r="F38" t="s" s="1883">
+      <c r="F38" t="s" s="2213">
         <v>44</v>
       </c>
-      <c r="G38" t="s" s="1880">
-        <v>215</v>
-      </c>
-      <c r="H38" t="s" s="1880">
+      <c r="G38" t="s" s="2210">
+        <v>223</v>
+      </c>
+      <c r="H38" t="s" s="2210">
         <v>46</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s" s="1748">
+      <c r="A39" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B39" t="s" s="1750">
+      <c r="B39" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C39" t="s" s="1884">
+      <c r="C39" t="s" s="2214">
         <v>179</v>
       </c>
-      <c r="D39" t="s" s="1885">
+      <c r="D39" t="s" s="2215">
         <v>25</v>
       </c>
-      <c r="E39" t="s" s="1886">
+      <c r="E39" t="s" s="2216">
         <v>44</v>
       </c>
-      <c r="F39" t="s" s="1887">
+      <c r="F39" t="s" s="2217">
         <v>44</v>
       </c>
-      <c r="G39" t="s" s="1884">
-        <v>215</v>
-      </c>
-      <c r="H39" t="s" s="1884">
+      <c r="G39" t="s" s="2214">
+        <v>223</v>
+      </c>
+      <c r="H39" t="s" s="2214">
         <v>46</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s" s="1748">
+      <c r="A40" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B40" t="s" s="1750">
+      <c r="B40" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C40" t="s" s="1888">
+      <c r="C40" t="s" s="2218">
         <v>180</v>
       </c>
-      <c r="D40" t="s" s="1889">
+      <c r="D40" t="s" s="2219">
         <v>25</v>
       </c>
-      <c r="E40" t="s" s="1890">
+      <c r="E40" t="s" s="2220">
         <v>44</v>
       </c>
-      <c r="F40" t="s" s="1891">
+      <c r="F40" t="s" s="2221">
         <v>44</v>
       </c>
-      <c r="G40" t="s" s="1888">
-        <v>215</v>
-      </c>
-      <c r="H40" t="s" s="1888">
+      <c r="G40" t="s" s="2218">
+        <v>223</v>
+      </c>
+      <c r="H40" t="s" s="2218">
         <v>46</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s" s="1748">
+      <c r="A41" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B41" t="s" s="1750">
+      <c r="B41" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C41" t="s" s="1892">
+      <c r="C41" t="s" s="2222">
         <v>181</v>
       </c>
-      <c r="D41" t="s" s="1893">
+      <c r="D41" t="s" s="2223">
         <v>25</v>
       </c>
-      <c r="E41" t="s" s="1894">
+      <c r="E41" t="s" s="2224">
         <v>44</v>
       </c>
-      <c r="F41" t="s" s="1895">
+      <c r="F41" t="s" s="2225">
         <v>44</v>
       </c>
-      <c r="G41" t="s" s="1892">
-        <v>215</v>
-      </c>
-      <c r="H41" t="s" s="1892">
+      <c r="G41" t="s" s="2222">
+        <v>223</v>
+      </c>
+      <c r="H41" t="s" s="2222">
         <v>46</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s" s="1748">
+      <c r="A42" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B42" t="s" s="1750">
+      <c r="B42" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C42" t="s" s="1896">
+      <c r="C42" t="s" s="2226">
         <v>182</v>
       </c>
-      <c r="D42" t="s" s="1897">
+      <c r="D42" t="s" s="2227">
         <v>25</v>
       </c>
-      <c r="E42" t="s" s="1898">
+      <c r="E42" t="s" s="2228">
         <v>44</v>
       </c>
-      <c r="F42" t="s" s="1899">
+      <c r="F42" t="s" s="2229">
         <v>44</v>
       </c>
-      <c r="G42" t="s" s="1896">
-        <v>215</v>
-      </c>
-      <c r="H42" t="s" s="1896">
+      <c r="G42" t="s" s="2226">
+        <v>223</v>
+      </c>
+      <c r="H42" t="s" s="2226">
         <v>46</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s" s="1748">
+      <c r="A43" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B43" t="s" s="1750">
+      <c r="B43" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C43" t="s" s="1900">
+      <c r="C43" t="s" s="2230">
         <v>183</v>
       </c>
-      <c r="D43" t="s" s="1901">
+      <c r="D43" t="s" s="2231">
         <v>25</v>
       </c>
-      <c r="E43" t="s" s="1902">
+      <c r="E43" t="s" s="2232">
         <v>44</v>
       </c>
-      <c r="F43" t="s" s="1903">
+      <c r="F43" t="s" s="2233">
         <v>44</v>
       </c>
-      <c r="G43" t="s" s="1900">
-        <v>215</v>
-      </c>
-      <c r="H43" t="s" s="1900">
+      <c r="G43" t="s" s="2230">
+        <v>223</v>
+      </c>
+      <c r="H43" t="s" s="2230">
         <v>46</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s" s="1748">
+      <c r="A44" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B44" t="s" s="1750">
+      <c r="B44" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C44" t="s" s="1904">
+      <c r="C44" t="s" s="2234">
         <v>185</v>
       </c>
-      <c r="D44" t="s" s="1905">
+      <c r="D44" t="s" s="2235">
         <v>25</v>
       </c>
-      <c r="E44" t="s" s="1906">
+      <c r="E44" t="s" s="2236">
         <v>44</v>
       </c>
-      <c r="F44" t="s" s="1907">
+      <c r="F44" t="s" s="2237">
         <v>44</v>
       </c>
-      <c r="G44" t="s" s="1904">
-        <v>215</v>
-      </c>
-      <c r="H44" t="s" s="1904">
+      <c r="G44" t="s" s="2234">
+        <v>223</v>
+      </c>
+      <c r="H44" t="s" s="2234">
         <v>46</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s" s="1748">
+      <c r="A45" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B45" t="s" s="1750">
+      <c r="B45" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C45" t="s" s="1908">
+      <c r="C45" t="s" s="2238">
         <v>186</v>
       </c>
-      <c r="D45" t="s" s="1909">
+      <c r="D45" t="s" s="2239">
         <v>25</v>
       </c>
-      <c r="E45" t="s" s="1910">
+      <c r="E45" t="s" s="2240">
         <v>44</v>
       </c>
-      <c r="F45" t="s" s="1911">
+      <c r="F45" t="s" s="2241">
         <v>44</v>
       </c>
-      <c r="G45" t="s" s="1908">
-        <v>215</v>
-      </c>
-      <c r="H45" t="s" s="1908">
+      <c r="G45" t="s" s="2238">
+        <v>223</v>
+      </c>
+      <c r="H45" t="s" s="2238">
         <v>46</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s" s="1748">
+      <c r="A46" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B46" t="s" s="1750">
+      <c r="B46" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C46" t="s" s="1912">
+      <c r="C46" t="s" s="2242">
         <v>188</v>
       </c>
-      <c r="D46" t="s" s="1913">
+      <c r="D46" t="s" s="2243">
         <v>25</v>
       </c>
-      <c r="E46" t="s" s="1914">
+      <c r="E46" t="s" s="2244">
         <v>44</v>
       </c>
-      <c r="F46" t="s" s="1915">
+      <c r="F46" t="s" s="2245">
         <v>44</v>
       </c>
-      <c r="G46" t="s" s="1912">
-        <v>215</v>
-      </c>
-      <c r="H46" t="s" s="1912">
+      <c r="G46" t="s" s="2242">
+        <v>223</v>
+      </c>
+      <c r="H46" t="s" s="2242">
         <v>46</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s" s="1748">
+      <c r="A47" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B47" t="s" s="1750">
+      <c r="B47" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C47" t="s" s="1916">
+      <c r="C47" t="s" s="2246">
         <v>190</v>
       </c>
-      <c r="D47" t="s" s="1917">
+      <c r="D47" t="s" s="2247">
         <v>25</v>
       </c>
-      <c r="E47" t="s" s="1918">
+      <c r="E47" t="s" s="2248">
         <v>44</v>
       </c>
-      <c r="F47" t="s" s="1919">
+      <c r="F47" t="s" s="2249">
         <v>44</v>
       </c>
-      <c r="G47" t="s" s="1916">
-        <v>215</v>
-      </c>
-      <c r="H47" t="s" s="1916">
+      <c r="G47" t="s" s="2246">
+        <v>223</v>
+      </c>
+      <c r="H47" t="s" s="2246">
         <v>46</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s" s="1748">
+      <c r="A48" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B48" t="s" s="1750">
+      <c r="B48" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C48" t="s" s="1920">
+      <c r="C48" t="s" s="2250">
         <v>192</v>
       </c>
-      <c r="D48" t="s" s="1921">
+      <c r="D48" t="s" s="2251">
         <v>25</v>
       </c>
-      <c r="E48" t="s" s="1922">
+      <c r="E48" t="s" s="2252">
         <v>44</v>
       </c>
-      <c r="F48" t="s" s="1923">
+      <c r="F48" t="s" s="2253">
         <v>44</v>
       </c>
-      <c r="G48" t="s" s="1920">
-        <v>215</v>
-      </c>
-      <c r="H48" t="s" s="1920">
+      <c r="G48" t="s" s="2250">
+        <v>223</v>
+      </c>
+      <c r="H48" t="s" s="2250">
         <v>46</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s" s="1748">
+      <c r="A49" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B49" t="s" s="1750">
+      <c r="B49" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C49" t="s" s="1924">
+      <c r="C49" t="s" s="2254">
         <v>193</v>
       </c>
-      <c r="D49" t="s" s="1925">
+      <c r="D49" t="s" s="2255">
         <v>25</v>
       </c>
-      <c r="E49" t="s" s="1926">
+      <c r="E49" t="s" s="2256">
         <v>44</v>
       </c>
-      <c r="F49" t="s" s="1927">
+      <c r="F49" t="s" s="2257">
         <v>44</v>
       </c>
-      <c r="G49" t="s" s="1924">
-        <v>215</v>
-      </c>
-      <c r="H49" t="s" s="1924">
+      <c r="G49" t="s" s="2254">
+        <v>223</v>
+      </c>
+      <c r="H49" t="s" s="2254">
         <v>46</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s" s="1748">
+      <c r="A50" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B50" t="s" s="1750">
+      <c r="B50" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C50" t="s" s="1928">
+      <c r="C50" t="s" s="2258">
         <v>194</v>
       </c>
-      <c r="D50" t="s" s="1929">
+      <c r="D50" t="s" s="2259">
         <v>25</v>
       </c>
-      <c r="E50" t="s" s="1930">
+      <c r="E50" t="s" s="2260">
         <v>44</v>
       </c>
-      <c r="F50" t="s" s="1931">
+      <c r="F50" t="s" s="2261">
         <v>44</v>
       </c>
-      <c r="G50" t="s" s="1928">
-        <v>215</v>
-      </c>
-      <c r="H50" t="s" s="1928">
+      <c r="G50" t="s" s="2258">
+        <v>223</v>
+      </c>
+      <c r="H50" t="s" s="2258">
         <v>46</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s" s="1748">
+      <c r="A51" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B51" t="s" s="1750">
+      <c r="B51" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C51" t="s" s="1932">
+      <c r="C51" t="s" s="2262">
         <v>195</v>
       </c>
-      <c r="D51" t="s" s="1933">
+      <c r="D51" t="s" s="2263">
         <v>25</v>
       </c>
-      <c r="E51" t="s" s="1934">
+      <c r="E51" t="s" s="2264">
         <v>44</v>
       </c>
-      <c r="F51" t="s" s="1935">
+      <c r="F51" t="s" s="2265">
         <v>44</v>
       </c>
-      <c r="G51" t="s" s="1932">
-        <v>215</v>
-      </c>
-      <c r="H51" t="s" s="1932">
+      <c r="G51" t="s" s="2262">
+        <v>223</v>
+      </c>
+      <c r="H51" t="s" s="2262">
         <v>46</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s" s="1748">
+      <c r="A52" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B52" t="s" s="1750">
+      <c r="B52" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C52" t="s" s="1936">
+      <c r="C52" t="s" s="2266">
         <v>196</v>
       </c>
-      <c r="D52" t="s" s="1937">
+      <c r="D52" t="s" s="2267">
         <v>25</v>
       </c>
-      <c r="E52" t="s" s="1938">
+      <c r="E52" t="s" s="2268">
         <v>44</v>
       </c>
-      <c r="F52" t="s" s="1939">
+      <c r="F52" t="s" s="2269">
         <v>44</v>
       </c>
-      <c r="G52" t="s" s="1936">
-        <v>215</v>
-      </c>
-      <c r="H52" t="s" s="1936">
+      <c r="G52" t="s" s="2266">
+        <v>223</v>
+      </c>
+      <c r="H52" t="s" s="2266">
         <v>46</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="s" s="1748">
+      <c r="A53" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B53" t="s" s="1750">
+      <c r="B53" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C53" t="s" s="1940">
+      <c r="C53" t="s" s="2270">
         <v>197</v>
       </c>
-      <c r="D53" t="s" s="1941">
+      <c r="D53" t="s" s="2271">
         <v>25</v>
       </c>
-      <c r="E53" t="s" s="1942">
+      <c r="E53" t="s" s="2272">
         <v>44</v>
       </c>
-      <c r="F53" t="s" s="1943">
+      <c r="F53" t="s" s="2273">
         <v>44</v>
       </c>
-      <c r="G53" t="s" s="1940">
-        <v>215</v>
-      </c>
-      <c r="H53" t="s" s="1940">
+      <c r="G53" t="s" s="2270">
+        <v>223</v>
+      </c>
+      <c r="H53" t="s" s="2270">
         <v>46</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="s" s="1748">
+      <c r="A54" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B54" t="s" s="1750">
+      <c r="B54" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C54" t="s" s="1944">
+      <c r="C54" t="s" s="2274">
         <v>216</v>
       </c>
-      <c r="D54" t="s" s="1945">
+      <c r="D54" t="s" s="2275">
         <v>25</v>
       </c>
-      <c r="E54" t="s" s="1946">
+      <c r="E54" t="s" s="2276">
         <v>44</v>
       </c>
-      <c r="F54" t="s" s="1947">
+      <c r="F54" t="s" s="2277">
         <v>44</v>
       </c>
-      <c r="G54" t="s" s="1944">
-        <v>215</v>
-      </c>
-      <c r="H54" t="s" s="1944">
+      <c r="G54" t="s" s="2274">
+        <v>223</v>
+      </c>
+      <c r="H54" t="s" s="2274">
         <v>46</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="s" s="1748">
+      <c r="A55" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B55" t="s" s="1750">
+      <c r="B55" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C55" t="s" s="1948">
+      <c r="C55" t="s" s="2278">
         <v>198</v>
       </c>
-      <c r="D55" t="s" s="1949">
+      <c r="D55" t="s" s="2279">
         <v>25</v>
       </c>
-      <c r="E55" t="s" s="1950">
+      <c r="E55" t="s" s="2280">
         <v>44</v>
       </c>
-      <c r="F55" t="s" s="1951">
+      <c r="F55" t="s" s="2281">
         <v>44</v>
       </c>
-      <c r="G55" t="s" s="1948">
-        <v>215</v>
-      </c>
-      <c r="H55" t="s" s="1948">
+      <c r="G55" t="s" s="2278">
+        <v>223</v>
+      </c>
+      <c r="H55" t="s" s="2278">
         <v>46</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="s" s="1748">
+      <c r="A56" t="s" s="2078">
         <v>176</v>
       </c>
-      <c r="B56" t="s" s="1750">
+      <c r="B56" t="s" s="2080">
         <v>177</v>
       </c>
-      <c r="C56" t="s" s="1952">
+      <c r="C56" t="s" s="2282">
         <v>199</v>
       </c>
-      <c r="D56" t="s" s="1953">
+      <c r="D56" t="s" s="2283">
         <v>25</v>
       </c>
-      <c r="E56" t="s" s="1954">
+      <c r="E56" t="s" s="2284">
         <v>44</v>
       </c>
-      <c r="F56" t="s" s="1955">
+      <c r="F56" t="s" s="2285">
         <v>44</v>
       </c>
-      <c r="G56" t="s" s="1952">
-        <v>215</v>
-      </c>
-      <c r="H56" t="s" s="1952">
+      <c r="G56" t="s" s="2282">
+        <v>223</v>
+      </c>
+      <c r="H56" t="s" s="2282">
         <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="69">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A13"/>

</xml_diff>